<commit_message>
* Added the difference and relative difference calculations.
</commit_message>
<xml_diff>
--- a/tests/data/desired/detailedreport.xlsx
+++ b/tests/data/desired/detailedreport.xlsx
@@ -15,19 +15,19 @@
     <sheet name="multicols" r:id="rId9" sheetId="7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">full!$B$2:$E$26</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">left!$B$2:$E$20</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="true">right!$B$2:$E$20</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="true">inner!$B$2:$E$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="true">diffs!$B$2:$E$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="true">append!$B$2:$E$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="true">multicols!$A$1:$F$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">full!$B$2:$G$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">left!$B$2:$G$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="true">right!$B$2:$G$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="true">inner!$B$2:$G$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="true">diffs!$B$2:$G$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="true">append!$B$2:$G$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="true">multicols!$A$1:$H$20</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="45">
   <si>
     <t>Column Name</t>
   </si>
@@ -41,6 +41,12 @@
     <t>Source2</t>
   </si>
   <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Relative</t>
+  </si>
+  <si>
     <t>FIRST_NAME</t>
   </si>
   <si>
@@ -50,6 +56,12 @@
     <t>2Bruce1</t>
   </si>
   <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>LAST_NAME</t>
   </si>
   <si>
@@ -62,6 +74,12 @@
     <t>AGE</t>
   </si>
   <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>47.62%</t>
+  </si>
+  <si>
     <t>1Martin2</t>
   </si>
   <si>
@@ -74,12 +92,18 @@
     <t>2Abone2</t>
   </si>
   <si>
+    <t>45.45%</t>
+  </si>
+  <si>
     <t>1Martin3</t>
   </si>
   <si>
     <t>1Velky3</t>
   </si>
   <si>
+    <t>100%</t>
+  </si>
+  <si>
     <t>2Bruce4</t>
   </si>
   <si>
@@ -101,13 +125,28 @@
     <t>Martin7</t>
   </si>
   <si>
+    <t>no</t>
+  </si>
+  <si>
     <t>Velky7</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>0.00%</t>
+  </si>
+  <si>
     <t>Bruce8</t>
   </si>
   <si>
     <t>Abone8</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>82.95%</t>
   </si>
   <si>
     <t>ACO</t>
@@ -130,7 +169,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="93">
+  <fonts count="151">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -233,6 +272,354 @@
       <name val="Calibri"/>
       <sz val="11.0"/>
       <color rgb="20D020"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="20D020"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="20D020"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="20D020"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="20D020"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="20D020"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="20D020"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="20D020"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="20D020"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="20D020"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="20D020"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="20D020"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="20D020"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="20D020"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="20D020"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
       <u val="none"/>
     </font>
     <font>
@@ -745,7 +1132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
@@ -840,6 +1227,64 @@
     <xf numFmtId="0" fontId="90" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="91" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="92" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="93" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="94" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="95" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="96" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="97" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="98" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="99" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="100" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="101" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="102" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="103" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="104" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="105" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="106" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="107" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="108" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="109" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="110" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="111" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="112" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="113" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="114" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="115" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="116" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="117" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="118" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="119" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="120" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="121" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="122" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="123" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="124" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="125" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="126" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="127" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="128" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="129" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="130" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="131" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="132" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="133" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="134" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="135" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="136" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="137" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="138" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="139" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="140" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="141" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="142" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="143" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="144" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="145" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="146" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="147" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="148" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="149" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="150" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -856,6 +1301,8 @@
     <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.78125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="12.9140625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="12.4609375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -871,38 +1318,56 @@
       <c r="E2" t="s" s="1">
         <v>3</v>
       </c>
+      <c r="F2" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="3">
       <c r="B3" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
         <v>1.0</v>
       </c>
       <c r="D3" t="s" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s" s="3">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="F3" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s" s="3">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
         <v>1.0</v>
       </c>
       <c r="D4" t="s" s="3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s" s="3">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="F4" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s" s="3">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
         <v>1.0</v>
@@ -913,38 +1378,56 @@
       <c r="E5" t="n" s="3">
         <v>21.0</v>
       </c>
+      <c r="F5" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s" s="3">
+        <v>16</v>
+      </c>
     </row>
     <row r="6">
       <c r="B6" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" t="n">
         <v>2.0</v>
       </c>
       <c r="D6" t="s" s="3">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s" s="3">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="F6" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s" s="3">
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C7" t="n">
         <v>2.0</v>
       </c>
       <c r="D7" t="s" s="3">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s" s="3">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="F7" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s" s="3">
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C8" t="n">
         <v>2.0</v>
@@ -955,32 +1438,44 @@
       <c r="E8" t="n" s="3">
         <v>22.0</v>
       </c>
+      <c r="F8" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s" s="3">
+        <v>21</v>
+      </c>
     </row>
     <row r="9">
       <c r="B9" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C9" t="n" s="3">
         <v>3.0</v>
       </c>
       <c r="D9" t="s" s="3">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="F9" t="s" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C10" t="n" s="3">
         <v>3.0</v>
       </c>
       <c r="D10" t="s" s="3">
-        <v>16</v>
+        <v>23</v>
+      </c>
+      <c r="F10" t="s" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C11" t="n" s="3">
         <v>3.0</v>
@@ -988,32 +1483,44 @@
       <c r="D11" t="n" s="3">
         <v>13.0</v>
       </c>
+      <c r="F11" t="n" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="G11" t="s" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="12">
       <c r="B12" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n" s="3">
         <v>4.0</v>
       </c>
       <c r="E12" t="s" s="3">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="F12" t="s" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C13" t="n" s="3">
         <v>4.0</v>
       </c>
       <c r="E13" t="s" s="3">
-        <v>18</v>
+        <v>26</v>
+      </c>
+      <c r="F13" t="s" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C14" t="n" s="3">
         <v>4.0</v>
@@ -1021,32 +1528,44 @@
       <c r="E14" t="n" s="3">
         <v>24.0</v>
       </c>
+      <c r="F14" t="n" s="3">
+        <v>24.0</v>
+      </c>
+      <c r="G14" t="s" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="15">
       <c r="B15" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C15" t="n" s="3">
         <v>5.0</v>
       </c>
       <c r="D15" t="s" s="3">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="F15" t="s" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C16" t="n" s="3">
         <v>5.0</v>
       </c>
       <c r="D16" t="s" s="3">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="F16" t="s" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C17" t="n" s="3">
         <v>5.0</v>
@@ -1054,32 +1573,44 @@
       <c r="D17" t="n" s="3">
         <v>15.0</v>
       </c>
+      <c r="F17" t="n" s="3">
+        <v>15.0</v>
+      </c>
+      <c r="G17" t="s" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="18">
       <c r="B18" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C18" t="n" s="3">
         <v>6.0</v>
       </c>
       <c r="E18" t="s" s="3">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="F18" t="s" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C19" t="n" s="3">
         <v>6.0</v>
       </c>
       <c r="E19" t="s" s="3">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="F19" t="s" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C20" t="n" s="3">
         <v>6.0</v>
@@ -1087,38 +1618,56 @@
       <c r="E20" t="n" s="3">
         <v>26.0</v>
       </c>
+      <c r="F20" t="n" s="3">
+        <v>26.0</v>
+      </c>
+      <c r="G20" t="s" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="21">
       <c r="B21" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C21" t="n">
         <v>7.0</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="F21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C22" t="n">
         <v>7.0</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>33</v>
+      </c>
+      <c r="F22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C23" t="n">
         <v>7.0</v>
@@ -1129,38 +1678,56 @@
       <c r="E23" t="n">
         <v>77.0</v>
       </c>
+      <c r="F23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="24">
       <c r="B24" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C24" t="n">
         <v>8.0</v>
       </c>
       <c r="D24" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="F24" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C25" t="n">
         <v>8.0</v>
       </c>
       <c r="D25" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E25" t="s">
-        <v>26</v>
+        <v>37</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C26" t="n">
         <v>8.0</v>
@@ -1171,9 +1738,15 @@
       <c r="E26" t="n" s="3">
         <v>88.0</v>
       </c>
+      <c r="F26" t="s" s="3">
+        <v>38</v>
+      </c>
+      <c r="G26" t="s" s="3">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:E26"/>
+  <autoFilter ref="B2:G26"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -1190,6 +1763,8 @@
     <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.78125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="12.9140625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="12.4609375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -1205,38 +1780,56 @@
       <c r="E2" t="s" s="1">
         <v>3</v>
       </c>
+      <c r="F2" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="3">
       <c r="B3" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
         <v>1.0</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
         <v>1.0</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
         <v>1.0</v>
@@ -1247,38 +1840,56 @@
       <c r="E5" t="n">
         <v>21.0</v>
       </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6">
       <c r="B6" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" t="n">
         <v>2.0</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C7" t="n">
         <v>2.0</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C8" t="n">
         <v>2.0</v>
@@ -1289,32 +1900,44 @@
       <c r="E8" t="n">
         <v>22.0</v>
       </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9">
       <c r="B9" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C9" t="n">
         <v>3.0</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C10" t="n">
         <v>3.0</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C11" t="n">
         <v>3.0</v>
@@ -1322,32 +1945,44 @@
       <c r="D11" t="n">
         <v>13.0</v>
       </c>
+      <c r="F11" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12">
       <c r="B12" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n">
         <v>5.0</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C13" t="n">
         <v>5.0</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C14" t="n">
         <v>5.0</v>
@@ -1355,38 +1990,56 @@
       <c r="D14" t="n">
         <v>15.0</v>
       </c>
+      <c r="F14" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15">
       <c r="B15" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C15" t="n">
         <v>7.0</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="F15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C16" t="n">
         <v>7.0</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>33</v>
+      </c>
+      <c r="F16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C17" t="n">
         <v>7.0</v>
@@ -1397,38 +2050,56 @@
       <c r="E17" t="n">
         <v>77.0</v>
       </c>
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="18">
       <c r="B18" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C18" t="n">
         <v>8.0</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="F18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C19" t="n">
         <v>8.0</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>37</v>
+      </c>
+      <c r="F19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C20" t="n">
         <v>8.0</v>
@@ -1439,9 +2110,15 @@
       <c r="E20" t="n">
         <v>88.0</v>
       </c>
+      <c r="F20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:E20"/>
+  <autoFilter ref="B2:G20"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -1458,6 +2135,8 @@
     <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.78125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="12.9140625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="12.4609375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -1473,38 +2152,56 @@
       <c r="E2" t="s" s="1">
         <v>3</v>
       </c>
+      <c r="F2" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="3">
       <c r="B3" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
         <v>1.0</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
         <v>1.0</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
         <v>1.0</v>
@@ -1515,38 +2212,56 @@
       <c r="E5" t="n">
         <v>21.0</v>
       </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6">
       <c r="B6" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" t="n">
         <v>2.0</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C7" t="n">
         <v>2.0</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C8" t="n">
         <v>2.0</v>
@@ -1557,32 +2272,44 @@
       <c r="E8" t="n">
         <v>22.0</v>
       </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9">
       <c r="B9" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C9" t="n">
         <v>4.0</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C10" t="n">
         <v>4.0</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C11" t="n">
         <v>4.0</v>
@@ -1590,32 +2317,44 @@
       <c r="E11" t="n">
         <v>24.0</v>
       </c>
+      <c r="F11" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12">
       <c r="B12" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n">
         <v>6.0</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C13" t="n">
         <v>6.0</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C14" t="n">
         <v>6.0</v>
@@ -1623,38 +2362,56 @@
       <c r="E14" t="n">
         <v>26.0</v>
       </c>
+      <c r="F14" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15">
       <c r="B15" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C15" t="n">
         <v>7.0</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="F15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C16" t="n">
         <v>7.0</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>33</v>
+      </c>
+      <c r="F16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C17" t="n">
         <v>7.0</v>
@@ -1665,38 +2422,56 @@
       <c r="E17" t="n">
         <v>77.0</v>
       </c>
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="18">
       <c r="B18" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C18" t="n">
         <v>8.0</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="F18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C19" t="n">
         <v>8.0</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>37</v>
+      </c>
+      <c r="F19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C20" t="n">
         <v>8.0</v>
@@ -1707,9 +2482,15 @@
       <c r="E20" t="n">
         <v>88.0</v>
       </c>
+      <c r="F20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:E20"/>
+  <autoFilter ref="B2:G20"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -1726,6 +2507,8 @@
     <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.78125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="12.9140625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="12.4609375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -1741,38 +2524,56 @@
       <c r="E2" t="s" s="1">
         <v>3</v>
       </c>
+      <c r="F2" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="3">
       <c r="B3" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
         <v>1.0</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
         <v>1.0</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
         <v>1.0</v>
@@ -1783,38 +2584,56 @@
       <c r="E5" t="n">
         <v>21.0</v>
       </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6">
       <c r="B6" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" t="n">
         <v>2.0</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C7" t="n">
         <v>2.0</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C8" t="n">
         <v>2.0</v>
@@ -1825,38 +2644,56 @@
       <c r="E8" t="n">
         <v>22.0</v>
       </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9">
       <c r="B9" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C9" t="n">
         <v>7.0</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C10" t="n">
         <v>7.0</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C11" t="n">
         <v>7.0</v>
@@ -1867,38 +2704,56 @@
       <c r="E11" t="n">
         <v>77.0</v>
       </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12">
       <c r="B12" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n">
         <v>8.0</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C13" t="n">
         <v>8.0</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>37</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C14" t="n">
         <v>8.0</v>
@@ -1908,6 +2763,12 @@
       </c>
       <c r="E14" t="n">
         <v>88.0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="20">
@@ -1923,38 +2784,56 @@
       <c r="E20" t="s" s="1">
         <v>2</v>
       </c>
+      <c r="F20" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="G20" t="s" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="21">
       <c r="B21" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C21" t="n">
         <v>1.0</v>
       </c>
       <c r="D21" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="F21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C22" t="n">
         <v>1.0</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="F22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C23" t="n">
         <v>1.0</v>
@@ -1965,38 +2844,56 @@
       <c r="E23" t="n">
         <v>11.0</v>
       </c>
+      <c r="F23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="24">
       <c r="B24" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C24" t="n">
         <v>2.0</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="F24" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C25" t="n">
         <v>2.0</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C26" t="n">
         <v>2.0</v>
@@ -2007,38 +2904,56 @@
       <c r="E26" t="n">
         <v>12.0</v>
       </c>
+      <c r="F26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="27">
       <c r="B27" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C27" t="n">
         <v>3.0</v>
       </c>
       <c r="D27" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="F27" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C28" t="n">
         <v>3.0</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E28" t="s">
-        <v>16</v>
+        <v>23</v>
+      </c>
+      <c r="F28" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C29" t="n">
         <v>3.0</v>
@@ -2049,38 +2964,56 @@
       <c r="E29" t="n">
         <v>13.0</v>
       </c>
+      <c r="F29" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="30">
       <c r="B30" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C30" t="n">
         <v>5.0</v>
       </c>
       <c r="D30" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E30" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="F30" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C31" t="n">
         <v>5.0</v>
       </c>
       <c r="D31" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E31" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="F31" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C32" t="n">
         <v>5.0</v>
@@ -2091,38 +3024,56 @@
       <c r="E32" t="n">
         <v>15.0</v>
       </c>
+      <c r="F32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="33">
       <c r="B33" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C33" t="n">
         <v>7.0</v>
       </c>
       <c r="D33" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E33" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="F33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G33" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C34" t="n">
         <v>7.0</v>
       </c>
       <c r="D34" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E34" t="s">
-        <v>24</v>
+        <v>33</v>
+      </c>
+      <c r="F34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G34" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C35" t="n">
         <v>7.0</v>
@@ -2133,38 +3084,56 @@
       <c r="E35" t="n">
         <v>77.0</v>
       </c>
+      <c r="F35" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="36">
       <c r="B36" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C36" t="n">
         <v>8.0</v>
       </c>
       <c r="D36" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E36" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="F36" t="s">
+        <v>32</v>
+      </c>
+      <c r="G36" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C37" t="n">
         <v>8.0</v>
       </c>
       <c r="D37" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E37" t="s">
-        <v>26</v>
+        <v>37</v>
+      </c>
+      <c r="F37" t="s">
+        <v>32</v>
+      </c>
+      <c r="G37" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C38" t="n">
         <v>8.0</v>
@@ -2175,9 +3144,15 @@
       <c r="E38" t="n">
         <v>15.0</v>
       </c>
+      <c r="F38" t="s">
+        <v>34</v>
+      </c>
+      <c r="G38" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="B20:E38"/>
+  <autoFilter ref="B20:G38"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -2194,6 +3169,8 @@
     <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.78125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="12.9140625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="12.4609375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -2209,38 +3186,56 @@
       <c r="E2" t="s" s="1">
         <v>3</v>
       </c>
+      <c r="F2" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="3">
       <c r="B3" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
         <v>1.0</v>
       </c>
       <c r="D3" t="s" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s" s="3">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="F3" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s" s="3">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
         <v>1.0</v>
       </c>
       <c r="D4" t="s" s="3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s" s="3">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="F4" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s" s="3">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
         <v>1.0</v>
@@ -2251,38 +3246,56 @@
       <c r="E5" t="n" s="3">
         <v>21.0</v>
       </c>
+      <c r="F5" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s" s="3">
+        <v>16</v>
+      </c>
     </row>
     <row r="6">
       <c r="B6" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" t="n">
         <v>2.0</v>
       </c>
       <c r="D6" t="s" s="3">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s" s="3">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="F6" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s" s="3">
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C7" t="n">
         <v>2.0</v>
       </c>
       <c r="D7" t="s" s="3">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s" s="3">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="F7" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s" s="3">
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C8" t="n">
         <v>2.0</v>
@@ -2293,32 +3306,44 @@
       <c r="E8" t="n" s="3">
         <v>22.0</v>
       </c>
+      <c r="F8" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s" s="3">
+        <v>21</v>
+      </c>
     </row>
     <row r="9">
       <c r="B9" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C9" t="n" s="3">
         <v>3.0</v>
       </c>
       <c r="D9" t="s" s="3">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="F9" t="s" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C10" t="n" s="3">
         <v>3.0</v>
       </c>
       <c r="D10" t="s" s="3">
-        <v>16</v>
+        <v>23</v>
+      </c>
+      <c r="F10" t="s" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C11" t="n" s="3">
         <v>3.0</v>
@@ -2326,32 +3351,44 @@
       <c r="D11" t="n" s="3">
         <v>13.0</v>
       </c>
+      <c r="F11" t="n" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="G11" t="s" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="12">
       <c r="B12" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n" s="3">
         <v>4.0</v>
       </c>
       <c r="E12" t="s" s="3">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="F12" t="s" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C13" t="n" s="3">
         <v>4.0</v>
       </c>
       <c r="E13" t="s" s="3">
-        <v>18</v>
+        <v>26</v>
+      </c>
+      <c r="F13" t="s" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C14" t="n" s="3">
         <v>4.0</v>
@@ -2359,32 +3396,44 @@
       <c r="E14" t="n" s="3">
         <v>24.0</v>
       </c>
+      <c r="F14" t="n" s="3">
+        <v>24.0</v>
+      </c>
+      <c r="G14" t="s" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="15">
       <c r="B15" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C15" t="n" s="3">
         <v>5.0</v>
       </c>
       <c r="D15" t="s" s="3">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="F15" t="s" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C16" t="n" s="3">
         <v>5.0</v>
       </c>
       <c r="D16" t="s" s="3">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="F16" t="s" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C17" t="n" s="3">
         <v>5.0</v>
@@ -2392,32 +3441,44 @@
       <c r="D17" t="n" s="3">
         <v>15.0</v>
       </c>
+      <c r="F17" t="n" s="3">
+        <v>15.0</v>
+      </c>
+      <c r="G17" t="s" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="18">
       <c r="B18" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C18" t="n" s="3">
         <v>6.0</v>
       </c>
       <c r="E18" t="s" s="3">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="F18" t="s" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C19" t="n" s="3">
         <v>6.0</v>
       </c>
       <c r="E19" t="s" s="3">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="F19" t="s" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C20" t="n" s="3">
         <v>6.0</v>
@@ -2425,10 +3486,16 @@
       <c r="E20" t="n" s="3">
         <v>26.0</v>
       </c>
+      <c r="F20" t="n" s="3">
+        <v>26.0</v>
+      </c>
+      <c r="G20" t="s" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="21">
       <c r="B21" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C21" t="n">
         <v>8.0</v>
@@ -2439,9 +3506,15 @@
       <c r="E21" t="n" s="3">
         <v>88.0</v>
       </c>
+      <c r="F21" t="s" s="3">
+        <v>38</v>
+      </c>
+      <c r="G21" t="s" s="3">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:E21"/>
+  <autoFilter ref="B2:G21"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -2458,6 +3531,8 @@
     <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.78125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="12.9140625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="12.4609375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -2473,205 +3548,295 @@
       <c r="E2" t="s" s="1">
         <v>3</v>
       </c>
+      <c r="F2" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="3">
       <c r="B3" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
         <v>1.0</v>
       </c>
       <c r="D3" t="s" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s" s="5">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="F3" t="s" s="6">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s" s="7">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
         <v>1.0</v>
       </c>
-      <c r="D4" t="s" s="6">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s" s="7">
-        <v>9</v>
+      <c r="D4" t="s" s="8">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s" s="9">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s" s="10">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s" s="11">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
         <v>1.0</v>
       </c>
-      <c r="D5" t="n" s="8">
+      <c r="D5" t="n" s="12">
         <v>11.0</v>
       </c>
-      <c r="E5" t="n" s="9">
+      <c r="E5" t="n" s="13">
         <v>21.0</v>
+      </c>
+      <c r="F5" t="s" s="14">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s" s="15">
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" t="n">
         <v>2.0</v>
       </c>
-      <c r="D6" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s" s="11">
-        <v>12</v>
+      <c r="D6" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s" s="17">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s" s="18">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s" s="19">
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C7" t="n">
         <v>2.0</v>
       </c>
-      <c r="D7" t="s" s="12">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s" s="13">
-        <v>14</v>
+      <c r="D7" t="s" s="20">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s" s="21">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s" s="22">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s" s="23">
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C8" t="n">
         <v>2.0</v>
       </c>
-      <c r="D8" t="n" s="14">
+      <c r="D8" t="n" s="24">
         <v>12.0</v>
       </c>
-      <c r="E8" t="n" s="15">
+      <c r="E8" t="n" s="25">
         <v>22.0</v>
+      </c>
+      <c r="F8" t="s" s="26">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s" s="27">
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C9" t="n">
         <v>8.0</v>
       </c>
-      <c r="D9" t="n" s="16">
+      <c r="D9" t="n" s="28">
         <v>15.0</v>
       </c>
-      <c r="E9" t="n" s="17">
+      <c r="E9" t="n" s="29">
         <v>88.0</v>
+      </c>
+      <c r="F9" t="s" s="30">
+        <v>38</v>
+      </c>
+      <c r="G9" t="s" s="31">
+        <v>39</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C10" t="n">
         <v>1.0</v>
       </c>
-      <c r="D10" t="s" s="18">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s" s="19">
-        <v>6</v>
+      <c r="D10" t="s" s="32">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s" s="33">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s" s="34">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s" s="35">
+        <v>10</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C11" t="n">
         <v>1.0</v>
       </c>
-      <c r="D11" t="s" s="20">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s" s="21">
-        <v>9</v>
+      <c r="D11" t="s" s="36">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s" s="37">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s" s="38">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s" s="39">
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C12" t="n">
         <v>1.0</v>
       </c>
-      <c r="D12" t="n" s="22">
+      <c r="D12" t="n" s="40">
         <v>11.0</v>
       </c>
-      <c r="E12" t="n" s="23">
+      <c r="E12" t="n" s="41">
         <v>21.0</v>
+      </c>
+      <c r="F12" t="s" s="42">
+        <v>15</v>
+      </c>
+      <c r="G12" t="s" s="43">
+        <v>16</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C13" t="n">
         <v>2.0</v>
       </c>
-      <c r="D13" t="s" s="24">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s" s="25">
-        <v>12</v>
+      <c r="D13" t="s" s="44">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s" s="45">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s" s="46">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s" s="47">
+        <v>10</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C14" t="n">
         <v>2.0</v>
       </c>
-      <c r="D14" t="s" s="26">
-        <v>13</v>
-      </c>
-      <c r="E14" t="s" s="27">
-        <v>14</v>
+      <c r="D14" t="s" s="48">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s" s="49">
+        <v>20</v>
+      </c>
+      <c r="F14" t="s" s="50">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s" s="51">
+        <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C15" t="n">
         <v>2.0</v>
       </c>
-      <c r="D15" t="n" s="28">
+      <c r="D15" t="n" s="52">
         <v>12.0</v>
       </c>
-      <c r="E15" t="n" s="29">
+      <c r="E15" t="n" s="53">
         <v>22.0</v>
+      </c>
+      <c r="F15" t="s" s="54">
+        <v>15</v>
+      </c>
+      <c r="G15" t="s" s="55">
+        <v>21</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C16" t="n">
         <v>8.0</v>
       </c>
-      <c r="D16" t="n" s="30">
+      <c r="D16" t="n" s="56">
         <v>15.0</v>
       </c>
-      <c r="E16" t="n" s="31">
+      <c r="E16" t="n" s="57">
         <v>88.0</v>
       </c>
+      <c r="F16" t="s" s="58">
+        <v>38</v>
+      </c>
+      <c r="G16" t="s" s="59">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:E16"/>
+  <autoFilter ref="B2:G16"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -2690,6 +3855,8 @@
     <col min="4" max="4" width="11.1484375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="12.78125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="12.9140625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.75390625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="12.4609375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2700,10 +3867,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s" s="1">
         <v>2</v>
@@ -2711,353 +3878,449 @@
       <c r="F1" t="s" s="1">
         <v>3</v>
       </c>
+      <c r="G1" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" t="n">
         <v>1.0</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s" s="32">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s" s="33">
-        <v>6</v>
+        <v>43</v>
+      </c>
+      <c r="E2" t="s" s="60">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s" s="61">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s" s="62">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s" s="63">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B3" t="n">
         <v>1.0</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s" s="34">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s" s="35">
-        <v>9</v>
+        <v>43</v>
+      </c>
+      <c r="E3" t="s" s="64">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s" s="65">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s" s="66">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s" s="67">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B4" t="n">
         <v>1.0</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" t="n" s="36">
+        <v>43</v>
+      </c>
+      <c r="E4" t="n" s="68">
         <v>11.0</v>
       </c>
-      <c r="F4" t="n" s="37">
+      <c r="F4" t="n" s="69">
         <v>21.0</v>
+      </c>
+      <c r="G4" t="s" s="70">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s" s="71">
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" t="n">
         <v>2.0</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" t="s" s="38">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s" s="39">
-        <v>12</v>
+        <v>43</v>
+      </c>
+      <c r="E5" t="s" s="72">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s" s="73">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s" s="74">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s" s="75">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>2.0</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" t="s" s="40">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s" s="41">
-        <v>14</v>
+        <v>43</v>
+      </c>
+      <c r="E6" t="s" s="76">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s" s="77">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s" s="78">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s" s="79">
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B7" t="n">
         <v>2.0</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" t="n" s="42">
+        <v>43</v>
+      </c>
+      <c r="E7" t="n" s="80">
         <v>12.0</v>
       </c>
-      <c r="F7" t="n" s="43">
+      <c r="F7" t="n" s="81">
         <v>22.0</v>
+      </c>
+      <c r="G7" t="s" s="82">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s" s="83">
+        <v>21</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>4</v>
-      </c>
-      <c r="B8" t="n" s="44">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n" s="84">
         <v>3.0</v>
       </c>
-      <c r="C8" t="s" s="45">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s" s="46">
-        <v>30</v>
-      </c>
-      <c r="E8" t="s" s="47">
-        <v>15</v>
+      <c r="C8" t="s" s="85">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s" s="86">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s" s="87">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s" s="88">
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n" s="48">
+        <v>11</v>
+      </c>
+      <c r="B9" t="n" s="89">
         <v>3.0</v>
       </c>
-      <c r="C9" t="s" s="49">
-        <v>29</v>
-      </c>
-      <c r="D9" t="s" s="50">
-        <v>30</v>
-      </c>
-      <c r="E9" t="s" s="51">
-        <v>16</v>
+      <c r="C9" t="s" s="90">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s" s="91">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s" s="92">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s" s="93">
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="B10" t="n" s="52">
+        <v>14</v>
+      </c>
+      <c r="B10" t="n" s="94">
         <v>3.0</v>
       </c>
-      <c r="C10" t="s" s="53">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s" s="54">
-        <v>30</v>
-      </c>
-      <c r="E10" t="n" s="55">
+      <c r="C10" t="s" s="95">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s" s="96">
+        <v>43</v>
+      </c>
+      <c r="E10" t="n" s="97">
         <v>13.0</v>
+      </c>
+      <c r="G10" t="n" s="98">
+        <v>13.0</v>
+      </c>
+      <c r="H10" t="s" s="99">
+        <v>24</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>4</v>
-      </c>
-      <c r="B11" t="n" s="56">
+        <v>6</v>
+      </c>
+      <c r="B11" t="n" s="100">
         <v>4.0</v>
       </c>
-      <c r="C11" t="s" s="57">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s" s="58">
-        <v>31</v>
-      </c>
-      <c r="F11" t="s" s="59">
-        <v>17</v>
+      <c r="C11" t="s" s="101">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s" s="102">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s" s="103">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s" s="104">
+        <v>9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="B12" t="n" s="60">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n" s="105">
         <v>4.0</v>
       </c>
-      <c r="C12" t="s" s="61">
-        <v>29</v>
-      </c>
-      <c r="D12" t="s" s="62">
-        <v>31</v>
-      </c>
-      <c r="F12" t="s" s="63">
-        <v>18</v>
+      <c r="C12" t="s" s="106">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s" s="107">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s" s="108">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s" s="109">
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="B13" t="n" s="64">
+        <v>14</v>
+      </c>
+      <c r="B13" t="n" s="110">
         <v>4.0</v>
       </c>
-      <c r="C13" t="s" s="65">
-        <v>29</v>
-      </c>
-      <c r="D13" t="s" s="66">
-        <v>31</v>
-      </c>
-      <c r="F13" t="n" s="67">
+      <c r="C13" t="s" s="111">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s" s="112">
+        <v>44</v>
+      </c>
+      <c r="F13" t="n" s="113">
         <v>24.0</v>
+      </c>
+      <c r="G13" t="n" s="114">
+        <v>24.0</v>
+      </c>
+      <c r="H13" t="s" s="115">
+        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>4</v>
-      </c>
-      <c r="B14" t="n" s="68">
+        <v>6</v>
+      </c>
+      <c r="B14" t="n" s="116">
         <v>5.0</v>
       </c>
-      <c r="C14" t="s" s="69">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s" s="70">
-        <v>30</v>
-      </c>
-      <c r="E14" t="s" s="71">
-        <v>19</v>
+      <c r="C14" t="s" s="117">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s" s="118">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s" s="119">
+        <v>27</v>
+      </c>
+      <c r="G14" t="s" s="120">
+        <v>9</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="B15" t="n" s="72">
+        <v>11</v>
+      </c>
+      <c r="B15" t="n" s="121">
         <v>5.0</v>
       </c>
-      <c r="C15" t="s" s="73">
-        <v>29</v>
-      </c>
-      <c r="D15" t="s" s="74">
-        <v>30</v>
-      </c>
-      <c r="E15" t="s" s="75">
-        <v>20</v>
+      <c r="C15" t="s" s="122">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s" s="123">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s" s="124">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s" s="125">
+        <v>9</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="B16" t="n" s="76">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n" s="126">
         <v>5.0</v>
       </c>
-      <c r="C16" t="s" s="77">
-        <v>29</v>
-      </c>
-      <c r="D16" t="s" s="78">
-        <v>30</v>
-      </c>
-      <c r="E16" t="n" s="79">
+      <c r="C16" t="s" s="127">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s" s="128">
+        <v>43</v>
+      </c>
+      <c r="E16" t="n" s="129">
         <v>15.0</v>
+      </c>
+      <c r="G16" t="n" s="130">
+        <v>15.0</v>
+      </c>
+      <c r="H16" t="s" s="131">
+        <v>24</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>4</v>
-      </c>
-      <c r="B17" t="n" s="80">
+        <v>6</v>
+      </c>
+      <c r="B17" t="n" s="132">
         <v>6.0</v>
       </c>
-      <c r="C17" t="s" s="81">
+      <c r="C17" t="s" s="133">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s" s="134">
+        <v>44</v>
+      </c>
+      <c r="F17" t="s" s="135">
         <v>29</v>
       </c>
-      <c r="D17" t="s" s="82">
-        <v>31</v>
-      </c>
-      <c r="F17" t="s" s="83">
-        <v>21</v>
+      <c r="G17" t="s" s="136">
+        <v>9</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="B18" t="n" s="84">
+        <v>11</v>
+      </c>
+      <c r="B18" t="n" s="137">
         <v>6.0</v>
       </c>
-      <c r="C18" t="s" s="85">
-        <v>29</v>
-      </c>
-      <c r="D18" t="s" s="86">
-        <v>31</v>
-      </c>
-      <c r="F18" t="s" s="87">
-        <v>22</v>
+      <c r="C18" t="s" s="138">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s" s="139">
+        <v>44</v>
+      </c>
+      <c r="F18" t="s" s="140">
+        <v>30</v>
+      </c>
+      <c r="G18" t="s" s="141">
+        <v>9</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="B19" t="n" s="88">
+        <v>14</v>
+      </c>
+      <c r="B19" t="n" s="142">
         <v>6.0</v>
       </c>
-      <c r="C19" t="s" s="89">
-        <v>29</v>
-      </c>
-      <c r="D19" t="s" s="90">
-        <v>31</v>
-      </c>
-      <c r="F19" t="n" s="91">
+      <c r="C19" t="s" s="143">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s" s="144">
+        <v>44</v>
+      </c>
+      <c r="F19" t="n" s="145">
         <v>26.0</v>
+      </c>
+      <c r="G19" t="n" s="146">
+        <v>26.0</v>
+      </c>
+      <c r="H19" t="s" s="147">
+        <v>24</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B20" t="n">
         <v>8.0</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" t="n" s="92">
+        <v>43</v>
+      </c>
+      <c r="E20" t="n" s="148">
         <v>15.0</v>
       </c>
-      <c r="F20" t="n" s="93">
+      <c r="F20" t="n" s="149">
         <v>88.0</v>
       </c>
+      <c r="G20" t="s" s="150">
+        <v>38</v>
+      </c>
+      <c r="H20" t="s" s="151">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F20"/>
+  <autoFilter ref="A1:H20"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* Extracted the BuilderInterface from ReportBuilder class. * Using double as data type for difference and relative difference calculations.
</commit_message>
<xml_diff>
--- a/tests/data/desired/detailedreport.xlsx
+++ b/tests/data/desired/detailedreport.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="37">
   <si>
     <t>Column Name</t>
   </si>
@@ -74,12 +74,6 @@
     <t>AGE</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>47.62%</t>
-  </si>
-  <si>
     <t>1Martin2</t>
   </si>
   <si>
@@ -92,16 +86,10 @@
     <t>2Abone2</t>
   </si>
   <si>
-    <t>45.45%</t>
-  </si>
-  <si>
     <t>1Martin3</t>
   </si>
   <si>
     <t>1Velky3</t>
-  </si>
-  <si>
-    <t>100%</t>
   </si>
   <si>
     <t>2Bruce4</t>
@@ -131,22 +119,10 @@
     <t>Velky7</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>0.00%</t>
-  </si>
-  <si>
     <t>Bruce8</t>
   </si>
   <si>
     <t>Abone8</t>
-  </si>
-  <si>
-    <t>73</t>
-  </si>
-  <si>
-    <t>82.95%</t>
   </si>
   <si>
     <t>ACO</t>
@@ -168,7 +144,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+  </numFmts>
   <fonts count="151">
     <font>
       <sz val="11.0"/>
@@ -1132,159 +1110,186 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+  <cellXfs count="179">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="33" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="34" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="35" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="36" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="37" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="38" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="41" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="42" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="43" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="46" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="47" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="48" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="49" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="50" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="51" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="52" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="53" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="54" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="56" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="57" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="59" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="60" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="61" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="62" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="63" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="64" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="65" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="66" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="67" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="68" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="69" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="70" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="71" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="72" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="73" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="74" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="75" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="76" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="77" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="78" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="79" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="80" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="81" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="82" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="83" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="84" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="85" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="86" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="87" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="88" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="89" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="90" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="91" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="92" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="93" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="94" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="95" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="96" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="97" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="98" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="99" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="100" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="101" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="102" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="103" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="104" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="105" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="106" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="107" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="108" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="109" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="110" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="111" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="112" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="113" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="114" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="115" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="116" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="117" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="118" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="119" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="120" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="121" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="122" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="123" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="124" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="125" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="126" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="127" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="128" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="129" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="130" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="131" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="132" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="133" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="134" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="135" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="136" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="137" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="138" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="139" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="140" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="141" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="142" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="143" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="144" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="145" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="146" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="147" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="148" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="149" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="150" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="26" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="30" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="33" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="34" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="34" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="35" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="36" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="37" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="38" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="38" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="41" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="42" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="42" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="43" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="46" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="46" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="47" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="48" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="49" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="50" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="50" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="51" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="52" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="53" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="54" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="54" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="56" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="57" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="58" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="59" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="61" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="62" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="62" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="63" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="64" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="65" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="66" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="66" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="67" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="68" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="69" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="70" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="70" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="71" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="72" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="73" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="74" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="74" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="75" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="76" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="77" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="78" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="78" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="79" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="80" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="81" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="82" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="82" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="83" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="84" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="85" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="86" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="87" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="88" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="89" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="90" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="91" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="92" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="93" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="94" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="95" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="96" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="97" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="98" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="98" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="99" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="100" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="101" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="102" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="103" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="104" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="105" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="106" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="107" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="108" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="109" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="110" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="111" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="112" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="113" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="114" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="114" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="115" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="116" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="117" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="118" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="119" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="120" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="121" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="122" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="123" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="124" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="125" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="126" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="127" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="128" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="129" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="130" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="130" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="131" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="132" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="133" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="134" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="135" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="136" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="137" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="138" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="139" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="140" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="141" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="142" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="143" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="144" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="145" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="146" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="146" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="147" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="148" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="149" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="150" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="150" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -1302,7 +1307,7 @@
     <col min="4" max="4" width="12.78125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="12.9140625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="12.4609375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="13.52734375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -1341,7 +1346,7 @@
       <c r="F3" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="G3" t="s" s="3">
+      <c r="G3" t="s" s="4">
         <v>10</v>
       </c>
     </row>
@@ -1361,7 +1366,7 @@
       <c r="F4" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="G4" t="s" s="3">
+      <c r="G4" t="s" s="4">
         <v>10</v>
       </c>
     </row>
@@ -1378,11 +1383,11 @@
       <c r="E5" t="n" s="3">
         <v>21.0</v>
       </c>
-      <c r="F5" t="s" s="3">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s" s="3">
-        <v>16</v>
+      <c r="F5" t="n" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="G5" t="n" s="4">
+        <v>0.47619047619047616</v>
       </c>
     </row>
     <row r="6">
@@ -1393,15 +1398,15 @@
         <v>2.0</v>
       </c>
       <c r="D6" t="s" s="3">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s" s="3">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="G6" t="s" s="3">
+      <c r="G6" t="s" s="4">
         <v>10</v>
       </c>
     </row>
@@ -1413,15 +1418,15 @@
         <v>2.0</v>
       </c>
       <c r="D7" t="s" s="3">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s" s="3">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="G7" t="s" s="3">
+      <c r="G7" t="s" s="4">
         <v>10</v>
       </c>
     </row>
@@ -1438,11 +1443,11 @@
       <c r="E8" t="n" s="3">
         <v>22.0</v>
       </c>
-      <c r="F8" t="s" s="3">
-        <v>15</v>
-      </c>
-      <c r="G8" t="s" s="3">
-        <v>21</v>
+      <c r="F8" t="n" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="G8" t="n" s="4">
+        <v>0.45454545454545453</v>
       </c>
     </row>
     <row r="9">
@@ -1453,7 +1458,7 @@
         <v>3.0</v>
       </c>
       <c r="D9" t="s" s="3">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s" s="3">
         <v>9</v>
@@ -1467,7 +1472,7 @@
         <v>3.0</v>
       </c>
       <c r="D10" t="s" s="3">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s" s="3">
         <v>9</v>
@@ -1486,8 +1491,8 @@
       <c r="F11" t="n" s="3">
         <v>13.0</v>
       </c>
-      <c r="G11" t="s" s="3">
-        <v>24</v>
+      <c r="G11" t="n" s="4">
+        <v>1.0</v>
       </c>
     </row>
     <row r="12">
@@ -1498,7 +1503,7 @@
         <v>4.0</v>
       </c>
       <c r="E12" t="s" s="3">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F12" t="s" s="3">
         <v>9</v>
@@ -1512,7 +1517,7 @@
         <v>4.0</v>
       </c>
       <c r="E13" t="s" s="3">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F13" t="s" s="3">
         <v>9</v>
@@ -1531,8 +1536,8 @@
       <c r="F14" t="n" s="3">
         <v>24.0</v>
       </c>
-      <c r="G14" t="s" s="3">
-        <v>24</v>
+      <c r="G14" t="n" s="4">
+        <v>1.0</v>
       </c>
     </row>
     <row r="15">
@@ -1543,7 +1548,7 @@
         <v>5.0</v>
       </c>
       <c r="D15" t="s" s="3">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F15" t="s" s="3">
         <v>9</v>
@@ -1557,7 +1562,7 @@
         <v>5.0</v>
       </c>
       <c r="D16" t="s" s="3">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F16" t="s" s="3">
         <v>9</v>
@@ -1576,8 +1581,8 @@
       <c r="F17" t="n" s="3">
         <v>15.0</v>
       </c>
-      <c r="G17" t="s" s="3">
-        <v>24</v>
+      <c r="G17" t="n" s="4">
+        <v>1.0</v>
       </c>
     </row>
     <row r="18">
@@ -1588,7 +1593,7 @@
         <v>6.0</v>
       </c>
       <c r="E18" t="s" s="3">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s" s="3">
         <v>9</v>
@@ -1602,7 +1607,7 @@
         <v>6.0</v>
       </c>
       <c r="E19" t="s" s="3">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F19" t="s" s="3">
         <v>9</v>
@@ -1621,8 +1626,8 @@
       <c r="F20" t="n" s="3">
         <v>26.0</v>
       </c>
-      <c r="G20" t="s" s="3">
-        <v>24</v>
+      <c r="G20" t="n" s="4">
+        <v>1.0</v>
       </c>
     </row>
     <row r="21">
@@ -1633,15 +1638,15 @@
         <v>7.0</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E21" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F21" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -1653,15 +1658,15 @@
         <v>7.0</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -1678,11 +1683,11 @@
       <c r="E23" t="n">
         <v>77.0</v>
       </c>
-      <c r="F23" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" t="s">
-        <v>35</v>
+      <c r="F23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G23" t="s" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="24">
@@ -1693,15 +1698,15 @@
         <v>8.0</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F24" t="s">
-        <v>32</v>
-      </c>
-      <c r="G24" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -1713,15 +1718,15 @@
         <v>8.0</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F25" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -1738,11 +1743,11 @@
       <c r="E26" t="n" s="3">
         <v>88.0</v>
       </c>
-      <c r="F26" t="s" s="3">
-        <v>38</v>
-      </c>
-      <c r="G26" t="s" s="3">
-        <v>39</v>
+      <c r="F26" t="n" s="3">
+        <v>73.0</v>
+      </c>
+      <c r="G26" t="n" s="4">
+        <v>0.8295454545454546</v>
       </c>
     </row>
   </sheetData>
@@ -1764,7 +1769,7 @@
     <col min="4" max="4" width="12.78125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="12.9140625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="12.4609375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="13.52734375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -1803,7 +1808,7 @@
       <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -1823,7 +1828,7 @@
       <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -1840,11 +1845,11 @@
       <c r="E5" t="n">
         <v>21.0</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
+      <c r="F5" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G5" t="n" s="5">
+        <v>0.47619047619047616</v>
       </c>
     </row>
     <row r="6">
@@ -1855,15 +1860,15 @@
         <v>2.0</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -1875,15 +1880,15 @@
         <v>2.0</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -1900,11 +1905,11 @@
       <c r="E8" t="n">
         <v>22.0</v>
       </c>
-      <c r="F8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
+      <c r="F8" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G8" t="n" s="5">
+        <v>0.45454545454545453</v>
       </c>
     </row>
     <row r="9">
@@ -1915,7 +1920,7 @@
         <v>3.0</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
         <v>9</v>
@@ -1929,7 +1934,7 @@
         <v>3.0</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
@@ -1948,8 +1953,8 @@
       <c r="F11" t="n">
         <v>13.0</v>
       </c>
-      <c r="G11" t="s">
-        <v>24</v>
+      <c r="G11" t="n" s="5">
+        <v>1.0</v>
       </c>
     </row>
     <row r="12">
@@ -1960,7 +1965,7 @@
         <v>5.0</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F12" t="s">
         <v>9</v>
@@ -1974,7 +1979,7 @@
         <v>5.0</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F13" t="s">
         <v>9</v>
@@ -1993,8 +1998,8 @@
       <c r="F14" t="n">
         <v>15.0</v>
       </c>
-      <c r="G14" t="s">
-        <v>24</v>
+      <c r="G14" t="n" s="5">
+        <v>1.0</v>
       </c>
     </row>
     <row r="15">
@@ -2005,15 +2010,15 @@
         <v>7.0</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2025,15 +2030,15 @@
         <v>7.0</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2050,11 +2055,11 @@
       <c r="E17" t="n">
         <v>77.0</v>
       </c>
-      <c r="F17" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" t="s">
-        <v>35</v>
+      <c r="F17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G17" t="s" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="18">
@@ -2065,15 +2070,15 @@
         <v>8.0</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F18" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2085,15 +2090,15 @@
         <v>8.0</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F19" t="s">
-        <v>32</v>
-      </c>
-      <c r="G19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2110,11 +2115,11 @@
       <c r="E20" t="n">
         <v>88.0</v>
       </c>
-      <c r="F20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" t="s">
-        <v>39</v>
+      <c r="F20" t="n">
+        <v>73.0</v>
+      </c>
+      <c r="G20" t="n" s="5">
+        <v>0.8295454545454546</v>
       </c>
     </row>
   </sheetData>
@@ -2136,7 +2141,7 @@
     <col min="4" max="4" width="12.78125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="12.9140625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="12.4609375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="13.52734375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -2175,7 +2180,7 @@
       <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2195,7 +2200,7 @@
       <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2212,11 +2217,11 @@
       <c r="E5" t="n">
         <v>21.0</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
+      <c r="F5" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G5" t="n" s="5">
+        <v>0.47619047619047616</v>
       </c>
     </row>
     <row r="6">
@@ -2227,15 +2232,15 @@
         <v>2.0</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2247,15 +2252,15 @@
         <v>2.0</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2272,11 +2277,11 @@
       <c r="E8" t="n">
         <v>22.0</v>
       </c>
-      <c r="F8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
+      <c r="F8" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G8" t="n" s="5">
+        <v>0.45454545454545453</v>
       </c>
     </row>
     <row r="9">
@@ -2287,7 +2292,7 @@
         <v>4.0</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F9" t="s">
         <v>9</v>
@@ -2301,7 +2306,7 @@
         <v>4.0</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
@@ -2320,8 +2325,8 @@
       <c r="F11" t="n">
         <v>24.0</v>
       </c>
-      <c r="G11" t="s">
-        <v>24</v>
+      <c r="G11" t="n" s="5">
+        <v>1.0</v>
       </c>
     </row>
     <row r="12">
@@ -2332,7 +2337,7 @@
         <v>6.0</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F12" t="s">
         <v>9</v>
@@ -2346,7 +2351,7 @@
         <v>6.0</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F13" t="s">
         <v>9</v>
@@ -2365,8 +2370,8 @@
       <c r="F14" t="n">
         <v>26.0</v>
       </c>
-      <c r="G14" t="s">
-        <v>24</v>
+      <c r="G14" t="n" s="5">
+        <v>1.0</v>
       </c>
     </row>
     <row r="15">
@@ -2377,15 +2382,15 @@
         <v>7.0</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2397,15 +2402,15 @@
         <v>7.0</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2422,11 +2427,11 @@
       <c r="E17" t="n">
         <v>77.0</v>
       </c>
-      <c r="F17" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" t="s">
-        <v>35</v>
+      <c r="F17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G17" t="s" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="18">
@@ -2437,15 +2442,15 @@
         <v>8.0</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F18" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2457,15 +2462,15 @@
         <v>8.0</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F19" t="s">
-        <v>32</v>
-      </c>
-      <c r="G19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2482,11 +2487,11 @@
       <c r="E20" t="n">
         <v>88.0</v>
       </c>
-      <c r="F20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" t="s">
-        <v>39</v>
+      <c r="F20" t="n">
+        <v>73.0</v>
+      </c>
+      <c r="G20" t="n" s="5">
+        <v>0.8295454545454546</v>
       </c>
     </row>
   </sheetData>
@@ -2508,7 +2513,7 @@
     <col min="4" max="4" width="12.78125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="12.9140625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="12.4609375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="12.55078125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -2547,7 +2552,7 @@
       <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2567,7 +2572,7 @@
       <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2584,11 +2589,11 @@
       <c r="E5" t="n">
         <v>21.0</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
+      <c r="F5" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G5" t="n" s="5">
+        <v>0.47619047619047616</v>
       </c>
     </row>
     <row r="6">
@@ -2599,15 +2604,15 @@
         <v>2.0</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2619,15 +2624,15 @@
         <v>2.0</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2644,11 +2649,11 @@
       <c r="E8" t="n">
         <v>22.0</v>
       </c>
-      <c r="F8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
+      <c r="F8" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G8" t="n" s="5">
+        <v>0.45454545454545453</v>
       </c>
     </row>
     <row r="9">
@@ -2659,15 +2664,15 @@
         <v>7.0</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2679,15 +2684,15 @@
         <v>7.0</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2704,11 +2709,11 @@
       <c r="E11" t="n">
         <v>77.0</v>
       </c>
-      <c r="F11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" t="s">
-        <v>35</v>
+      <c r="F11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G11" t="s" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -2719,15 +2724,15 @@
         <v>8.0</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2739,15 +2744,15 @@
         <v>8.0</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2764,11 +2769,11 @@
       <c r="E14" t="n">
         <v>88.0</v>
       </c>
-      <c r="F14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" t="s">
-        <v>39</v>
+      <c r="F14" t="n">
+        <v>73.0</v>
+      </c>
+      <c r="G14" t="n" s="5">
+        <v>0.8295454545454546</v>
       </c>
     </row>
     <row r="20">
@@ -2805,9 +2810,9 @@
         <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2825,9 +2830,9 @@
         <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2844,11 +2849,11 @@
       <c r="E23" t="n">
         <v>11.0</v>
       </c>
-      <c r="F23" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" t="s">
-        <v>35</v>
+      <c r="F23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G23" t="s" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="24">
@@ -2859,15 +2864,15 @@
         <v>2.0</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>32</v>
-      </c>
-      <c r="G24" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2879,15 +2884,15 @@
         <v>2.0</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F25" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2904,11 +2909,11 @@
       <c r="E26" t="n">
         <v>12.0</v>
       </c>
-      <c r="F26" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" t="s">
-        <v>35</v>
+      <c r="F26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G26" t="s" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="27">
@@ -2919,15 +2924,15 @@
         <v>3.0</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E27" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>32</v>
-      </c>
-      <c r="G27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2939,15 +2944,15 @@
         <v>3.0</v>
       </c>
       <c r="D28" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E28" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F28" t="s">
-        <v>32</v>
-      </c>
-      <c r="G28" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2964,11 +2969,11 @@
       <c r="E29" t="n">
         <v>13.0</v>
       </c>
-      <c r="F29" t="s">
-        <v>34</v>
-      </c>
-      <c r="G29" t="s">
-        <v>35</v>
+      <c r="F29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G29" t="s" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="30">
@@ -2979,15 +2984,15 @@
         <v>5.0</v>
       </c>
       <c r="D30" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E30" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F30" t="s">
-        <v>32</v>
-      </c>
-      <c r="G30" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2999,15 +3004,15 @@
         <v>5.0</v>
       </c>
       <c r="D31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" t="s">
         <v>28</v>
       </c>
-      <c r="E31" t="s">
-        <v>28</v>
-      </c>
-      <c r="F31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="G31" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -3024,11 +3029,11 @@
       <c r="E32" t="n">
         <v>15.0</v>
       </c>
-      <c r="F32" t="s">
-        <v>34</v>
-      </c>
-      <c r="G32" t="s">
-        <v>35</v>
+      <c r="F32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G32" t="s" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="33">
@@ -3039,15 +3044,15 @@
         <v>7.0</v>
       </c>
       <c r="D33" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E33" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F33" t="s">
-        <v>32</v>
-      </c>
-      <c r="G33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -3059,15 +3064,15 @@
         <v>7.0</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E34" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F34" t="s">
-        <v>32</v>
-      </c>
-      <c r="G34" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -3084,11 +3089,11 @@
       <c r="E35" t="n">
         <v>77.0</v>
       </c>
-      <c r="F35" t="s">
-        <v>34</v>
-      </c>
-      <c r="G35" t="s">
-        <v>35</v>
+      <c r="F35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G35" t="s" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="36">
@@ -3099,15 +3104,15 @@
         <v>8.0</v>
       </c>
       <c r="D36" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E36" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F36" t="s">
-        <v>32</v>
-      </c>
-      <c r="G36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -3119,15 +3124,15 @@
         <v>8.0</v>
       </c>
       <c r="D37" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E37" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F37" t="s">
-        <v>32</v>
-      </c>
-      <c r="G37" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -3144,11 +3149,11 @@
       <c r="E38" t="n">
         <v>15.0</v>
       </c>
-      <c r="F38" t="s">
-        <v>34</v>
-      </c>
-      <c r="G38" t="s">
-        <v>35</v>
+      <c r="F38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G38" t="s" s="5">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3170,7 +3175,7 @@
     <col min="4" max="4" width="12.78125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="12.9140625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="12.4609375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="13.52734375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -3209,7 +3214,7 @@
       <c r="F3" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="G3" t="s" s="3">
+      <c r="G3" t="s" s="4">
         <v>10</v>
       </c>
     </row>
@@ -3229,7 +3234,7 @@
       <c r="F4" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="G4" t="s" s="3">
+      <c r="G4" t="s" s="4">
         <v>10</v>
       </c>
     </row>
@@ -3246,11 +3251,11 @@
       <c r="E5" t="n" s="3">
         <v>21.0</v>
       </c>
-      <c r="F5" t="s" s="3">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s" s="3">
-        <v>16</v>
+      <c r="F5" t="n" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="G5" t="n" s="4">
+        <v>0.47619047619047616</v>
       </c>
     </row>
     <row r="6">
@@ -3261,15 +3266,15 @@
         <v>2.0</v>
       </c>
       <c r="D6" t="s" s="3">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s" s="3">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="G6" t="s" s="3">
+      <c r="G6" t="s" s="4">
         <v>10</v>
       </c>
     </row>
@@ -3281,15 +3286,15 @@
         <v>2.0</v>
       </c>
       <c r="D7" t="s" s="3">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s" s="3">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="G7" t="s" s="3">
+      <c r="G7" t="s" s="4">
         <v>10</v>
       </c>
     </row>
@@ -3306,11 +3311,11 @@
       <c r="E8" t="n" s="3">
         <v>22.0</v>
       </c>
-      <c r="F8" t="s" s="3">
-        <v>15</v>
-      </c>
-      <c r="G8" t="s" s="3">
-        <v>21</v>
+      <c r="F8" t="n" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="G8" t="n" s="4">
+        <v>0.45454545454545453</v>
       </c>
     </row>
     <row r="9">
@@ -3321,7 +3326,7 @@
         <v>3.0</v>
       </c>
       <c r="D9" t="s" s="3">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s" s="3">
         <v>9</v>
@@ -3335,7 +3340,7 @@
         <v>3.0</v>
       </c>
       <c r="D10" t="s" s="3">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s" s="3">
         <v>9</v>
@@ -3354,8 +3359,8 @@
       <c r="F11" t="n" s="3">
         <v>13.0</v>
       </c>
-      <c r="G11" t="s" s="3">
-        <v>24</v>
+      <c r="G11" t="n" s="4">
+        <v>1.0</v>
       </c>
     </row>
     <row r="12">
@@ -3366,7 +3371,7 @@
         <v>4.0</v>
       </c>
       <c r="E12" t="s" s="3">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F12" t="s" s="3">
         <v>9</v>
@@ -3380,7 +3385,7 @@
         <v>4.0</v>
       </c>
       <c r="E13" t="s" s="3">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F13" t="s" s="3">
         <v>9</v>
@@ -3399,8 +3404,8 @@
       <c r="F14" t="n" s="3">
         <v>24.0</v>
       </c>
-      <c r="G14" t="s" s="3">
-        <v>24</v>
+      <c r="G14" t="n" s="4">
+        <v>1.0</v>
       </c>
     </row>
     <row r="15">
@@ -3411,7 +3416,7 @@
         <v>5.0</v>
       </c>
       <c r="D15" t="s" s="3">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F15" t="s" s="3">
         <v>9</v>
@@ -3425,7 +3430,7 @@
         <v>5.0</v>
       </c>
       <c r="D16" t="s" s="3">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F16" t="s" s="3">
         <v>9</v>
@@ -3444,8 +3449,8 @@
       <c r="F17" t="n" s="3">
         <v>15.0</v>
       </c>
-      <c r="G17" t="s" s="3">
-        <v>24</v>
+      <c r="G17" t="n" s="4">
+        <v>1.0</v>
       </c>
     </row>
     <row r="18">
@@ -3456,7 +3461,7 @@
         <v>6.0</v>
       </c>
       <c r="E18" t="s" s="3">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s" s="3">
         <v>9</v>
@@ -3470,7 +3475,7 @@
         <v>6.0</v>
       </c>
       <c r="E19" t="s" s="3">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F19" t="s" s="3">
         <v>9</v>
@@ -3489,8 +3494,8 @@
       <c r="F20" t="n" s="3">
         <v>26.0</v>
       </c>
-      <c r="G20" t="s" s="3">
-        <v>24</v>
+      <c r="G20" t="n" s="4">
+        <v>1.0</v>
       </c>
     </row>
     <row r="21">
@@ -3506,11 +3511,11 @@
       <c r="E21" t="n" s="3">
         <v>88.0</v>
       </c>
-      <c r="F21" t="s" s="3">
-        <v>38</v>
-      </c>
-      <c r="G21" t="s" s="3">
-        <v>39</v>
+      <c r="F21" t="n" s="3">
+        <v>73.0</v>
+      </c>
+      <c r="G21" t="n" s="4">
+        <v>0.8295454545454546</v>
       </c>
     </row>
   </sheetData>
@@ -3532,7 +3537,7 @@
     <col min="4" max="4" width="12.78125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="12.9140625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="12.4609375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="12.55078125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -3562,16 +3567,16 @@
       <c r="C3" t="n">
         <v>1.0</v>
       </c>
-      <c r="D3" t="s" s="4">
+      <c r="D3" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="E3" t="s" s="5">
+      <c r="E3" t="s" s="7">
         <v>8</v>
       </c>
-      <c r="F3" t="s" s="6">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s" s="7">
+      <c r="F3" t="s" s="8">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s" s="10">
         <v>10</v>
       </c>
     </row>
@@ -3582,16 +3587,16 @@
       <c r="C4" t="n">
         <v>1.0</v>
       </c>
-      <c r="D4" t="s" s="8">
+      <c r="D4" t="s" s="11">
         <v>12</v>
       </c>
-      <c r="E4" t="s" s="9">
+      <c r="E4" t="s" s="12">
         <v>13</v>
       </c>
-      <c r="F4" t="s" s="10">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s" s="11">
+      <c r="F4" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s" s="15">
         <v>10</v>
       </c>
     </row>
@@ -3602,17 +3607,17 @@
       <c r="C5" t="n">
         <v>1.0</v>
       </c>
-      <c r="D5" t="n" s="12">
+      <c r="D5" t="n" s="16">
         <v>11.0</v>
       </c>
-      <c r="E5" t="n" s="13">
+      <c r="E5" t="n" s="17">
         <v>21.0</v>
       </c>
-      <c r="F5" t="s" s="14">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s" s="15">
-        <v>16</v>
+      <c r="F5" t="n" s="18">
+        <v>10.0</v>
+      </c>
+      <c r="G5" t="n" s="20">
+        <v>0.47619047619047616</v>
       </c>
     </row>
     <row r="6">
@@ -3622,16 +3627,16 @@
       <c r="C6" t="n">
         <v>2.0</v>
       </c>
-      <c r="D6" t="s" s="16">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s" s="17">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s" s="18">
-        <v>9</v>
-      </c>
-      <c r="G6" t="s" s="19">
+      <c r="D6" t="s" s="21">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s" s="22">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s" s="23">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s" s="25">
         <v>10</v>
       </c>
     </row>
@@ -3642,16 +3647,16 @@
       <c r="C7" t="n">
         <v>2.0</v>
       </c>
-      <c r="D7" t="s" s="20">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s" s="21">
-        <v>20</v>
-      </c>
-      <c r="F7" t="s" s="22">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s" s="23">
+      <c r="D7" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s" s="27">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s" s="28">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s" s="30">
         <v>10</v>
       </c>
     </row>
@@ -3662,17 +3667,17 @@
       <c r="C8" t="n">
         <v>2.0</v>
       </c>
-      <c r="D8" t="n" s="24">
+      <c r="D8" t="n" s="31">
         <v>12.0</v>
       </c>
-      <c r="E8" t="n" s="25">
+      <c r="E8" t="n" s="32">
         <v>22.0</v>
       </c>
-      <c r="F8" t="s" s="26">
-        <v>15</v>
-      </c>
-      <c r="G8" t="s" s="27">
-        <v>21</v>
+      <c r="F8" t="n" s="33">
+        <v>10.0</v>
+      </c>
+      <c r="G8" t="n" s="35">
+        <v>0.45454545454545453</v>
       </c>
     </row>
     <row r="9">
@@ -3682,17 +3687,17 @@
       <c r="C9" t="n">
         <v>8.0</v>
       </c>
-      <c r="D9" t="n" s="28">
+      <c r="D9" t="n" s="36">
         <v>15.0</v>
       </c>
-      <c r="E9" t="n" s="29">
+      <c r="E9" t="n" s="37">
         <v>88.0</v>
       </c>
-      <c r="F9" t="s" s="30">
-        <v>38</v>
-      </c>
-      <c r="G9" t="s" s="31">
-        <v>39</v>
+      <c r="F9" t="n" s="38">
+        <v>73.0</v>
+      </c>
+      <c r="G9" t="n" s="40">
+        <v>0.8295454545454546</v>
       </c>
     </row>
     <row r="10">
@@ -3702,16 +3707,16 @@
       <c r="C10" t="n">
         <v>1.0</v>
       </c>
-      <c r="D10" t="s" s="32">
+      <c r="D10" t="s" s="41">
         <v>7</v>
       </c>
-      <c r="E10" t="s" s="33">
+      <c r="E10" t="s" s="42">
         <v>8</v>
       </c>
-      <c r="F10" t="s" s="34">
-        <v>9</v>
-      </c>
-      <c r="G10" t="s" s="35">
+      <c r="F10" t="s" s="43">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s" s="45">
         <v>10</v>
       </c>
     </row>
@@ -3722,16 +3727,16 @@
       <c r="C11" t="n">
         <v>1.0</v>
       </c>
-      <c r="D11" t="s" s="36">
+      <c r="D11" t="s" s="46">
         <v>12</v>
       </c>
-      <c r="E11" t="s" s="37">
+      <c r="E11" t="s" s="47">
         <v>13</v>
       </c>
-      <c r="F11" t="s" s="38">
-        <v>9</v>
-      </c>
-      <c r="G11" t="s" s="39">
+      <c r="F11" t="s" s="48">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s" s="50">
         <v>10</v>
       </c>
     </row>
@@ -3742,17 +3747,17 @@
       <c r="C12" t="n">
         <v>1.0</v>
       </c>
-      <c r="D12" t="n" s="40">
+      <c r="D12" t="n" s="51">
         <v>11.0</v>
       </c>
-      <c r="E12" t="n" s="41">
+      <c r="E12" t="n" s="52">
         <v>21.0</v>
       </c>
-      <c r="F12" t="s" s="42">
-        <v>15</v>
-      </c>
-      <c r="G12" t="s" s="43">
-        <v>16</v>
+      <c r="F12" t="n" s="53">
+        <v>10.0</v>
+      </c>
+      <c r="G12" t="n" s="55">
+        <v>0.47619047619047616</v>
       </c>
     </row>
     <row r="13">
@@ -3762,16 +3767,16 @@
       <c r="C13" t="n">
         <v>2.0</v>
       </c>
-      <c r="D13" t="s" s="44">
-        <v>17</v>
-      </c>
-      <c r="E13" t="s" s="45">
-        <v>18</v>
-      </c>
-      <c r="F13" t="s" s="46">
-        <v>9</v>
-      </c>
-      <c r="G13" t="s" s="47">
+      <c r="D13" t="s" s="56">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s" s="57">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s" s="58">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s" s="60">
         <v>10</v>
       </c>
     </row>
@@ -3782,16 +3787,16 @@
       <c r="C14" t="n">
         <v>2.0</v>
       </c>
-      <c r="D14" t="s" s="48">
-        <v>19</v>
-      </c>
-      <c r="E14" t="s" s="49">
-        <v>20</v>
-      </c>
-      <c r="F14" t="s" s="50">
-        <v>9</v>
-      </c>
-      <c r="G14" t="s" s="51">
+      <c r="D14" t="s" s="61">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s" s="62">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s" s="63">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s" s="65">
         <v>10</v>
       </c>
     </row>
@@ -3802,17 +3807,17 @@
       <c r="C15" t="n">
         <v>2.0</v>
       </c>
-      <c r="D15" t="n" s="52">
+      <c r="D15" t="n" s="66">
         <v>12.0</v>
       </c>
-      <c r="E15" t="n" s="53">
+      <c r="E15" t="n" s="67">
         <v>22.0</v>
       </c>
-      <c r="F15" t="s" s="54">
-        <v>15</v>
-      </c>
-      <c r="G15" t="s" s="55">
-        <v>21</v>
+      <c r="F15" t="n" s="68">
+        <v>10.0</v>
+      </c>
+      <c r="G15" t="n" s="70">
+        <v>0.45454545454545453</v>
       </c>
     </row>
     <row r="16">
@@ -3822,17 +3827,17 @@
       <c r="C16" t="n">
         <v>8.0</v>
       </c>
-      <c r="D16" t="n" s="56">
+      <c r="D16" t="n" s="71">
         <v>15.0</v>
       </c>
-      <c r="E16" t="n" s="57">
+      <c r="E16" t="n" s="72">
         <v>88.0</v>
       </c>
-      <c r="F16" t="s" s="58">
-        <v>38</v>
-      </c>
-      <c r="G16" t="s" s="59">
-        <v>39</v>
+      <c r="F16" t="n" s="73">
+        <v>73.0</v>
+      </c>
+      <c r="G16" t="n" s="75">
+        <v>0.8295454545454546</v>
       </c>
     </row>
   </sheetData>
@@ -3856,7 +3861,7 @@
     <col min="5" max="5" width="12.78125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="12.9140625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.75390625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.4609375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.52734375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3867,10 +3872,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s" s="1">
         <v>2</v>
@@ -3893,21 +3898,21 @@
         <v>1.0</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" t="s" s="60">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s" s="76">
         <v>7</v>
       </c>
-      <c r="F2" t="s" s="61">
+      <c r="F2" t="s" s="77">
         <v>8</v>
       </c>
-      <c r="G2" t="s" s="62">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s" s="63">
+      <c r="G2" t="s" s="78">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s" s="80">
         <v>10</v>
       </c>
     </row>
@@ -3919,21 +3924,21 @@
         <v>1.0</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" t="s" s="64">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s" s="81">
         <v>12</v>
       </c>
-      <c r="F3" t="s" s="65">
+      <c r="F3" t="s" s="82">
         <v>13</v>
       </c>
-      <c r="G3" t="s" s="66">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s" s="67">
+      <c r="G3" t="s" s="83">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s" s="85">
         <v>10</v>
       </c>
     </row>
@@ -3945,22 +3950,22 @@
         <v>1.0</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" t="n" s="68">
+        <v>35</v>
+      </c>
+      <c r="E4" t="n" s="86">
         <v>11.0</v>
       </c>
-      <c r="F4" t="n" s="69">
+      <c r="F4" t="n" s="87">
         <v>21.0</v>
       </c>
-      <c r="G4" t="s" s="70">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s" s="71">
-        <v>16</v>
+      <c r="G4" t="n" s="88">
+        <v>10.0</v>
+      </c>
+      <c r="H4" t="n" s="90">
+        <v>0.47619047619047616</v>
       </c>
     </row>
     <row r="5">
@@ -3971,21 +3976,21 @@
         <v>2.0</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" t="s" s="72">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s" s="73">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s" s="74">
-        <v>9</v>
-      </c>
-      <c r="H5" t="s" s="75">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s" s="91">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s" s="92">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s" s="93">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s" s="95">
         <v>10</v>
       </c>
     </row>
@@ -3997,21 +4002,21 @@
         <v>2.0</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" t="s" s="76">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s" s="77">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s" s="78">
-        <v>9</v>
-      </c>
-      <c r="H6" t="s" s="79">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s" s="96">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s" s="97">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s" s="98">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s" s="100">
         <v>10</v>
       </c>
     </row>
@@ -4023,41 +4028,41 @@
         <v>2.0</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" t="n" s="80">
+        <v>35</v>
+      </c>
+      <c r="E7" t="n" s="101">
         <v>12.0</v>
       </c>
-      <c r="F7" t="n" s="81">
+      <c r="F7" t="n" s="102">
         <v>22.0</v>
       </c>
-      <c r="G7" t="s" s="82">
-        <v>15</v>
-      </c>
-      <c r="H7" t="s" s="83">
-        <v>21</v>
+      <c r="G7" t="n" s="103">
+        <v>10.0</v>
+      </c>
+      <c r="H7" t="n" s="105">
+        <v>0.45454545454545453</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="B8" t="n" s="84">
+      <c r="B8" t="n" s="106">
         <v>3.0</v>
       </c>
-      <c r="C8" t="s" s="85">
-        <v>42</v>
-      </c>
-      <c r="D8" t="s" s="86">
-        <v>43</v>
-      </c>
-      <c r="E8" t="s" s="87">
-        <v>22</v>
-      </c>
-      <c r="G8" t="s" s="88">
+      <c r="C8" t="s" s="107">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s" s="108">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s" s="109">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s" s="110">
         <v>9</v>
       </c>
     </row>
@@ -4065,19 +4070,19 @@
       <c r="A9" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="B9" t="n" s="89">
+      <c r="B9" t="n" s="111">
         <v>3.0</v>
       </c>
-      <c r="C9" t="s" s="90">
-        <v>42</v>
-      </c>
-      <c r="D9" t="s" s="91">
-        <v>43</v>
-      </c>
-      <c r="E9" t="s" s="92">
-        <v>23</v>
-      </c>
-      <c r="G9" t="s" s="93">
+      <c r="C9" t="s" s="112">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s" s="113">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s" s="114">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s" s="115">
         <v>9</v>
       </c>
     </row>
@@ -4085,42 +4090,42 @@
       <c r="A10" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="B10" t="n" s="94">
+      <c r="B10" t="n" s="116">
         <v>3.0</v>
       </c>
-      <c r="C10" t="s" s="95">
-        <v>42</v>
-      </c>
-      <c r="D10" t="s" s="96">
-        <v>43</v>
-      </c>
-      <c r="E10" t="n" s="97">
+      <c r="C10" t="s" s="117">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s" s="118">
+        <v>35</v>
+      </c>
+      <c r="E10" t="n" s="119">
         <v>13.0</v>
       </c>
-      <c r="G10" t="n" s="98">
+      <c r="G10" t="n" s="120">
         <v>13.0</v>
       </c>
-      <c r="H10" t="s" s="99">
-        <v>24</v>
+      <c r="H10" t="n" s="122">
+        <v>1.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="B11" t="n" s="100">
+      <c r="B11" t="n" s="123">
         <v>4.0</v>
       </c>
-      <c r="C11" t="s" s="101">
-        <v>42</v>
-      </c>
-      <c r="D11" t="s" s="102">
-        <v>44</v>
-      </c>
-      <c r="F11" t="s" s="103">
-        <v>25</v>
-      </c>
-      <c r="G11" t="s" s="104">
+      <c r="C11" t="s" s="124">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s" s="125">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s" s="126">
+        <v>21</v>
+      </c>
+      <c r="G11" t="s" s="127">
         <v>9</v>
       </c>
     </row>
@@ -4128,19 +4133,19 @@
       <c r="A12" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="B12" t="n" s="105">
+      <c r="B12" t="n" s="128">
         <v>4.0</v>
       </c>
-      <c r="C12" t="s" s="106">
-        <v>42</v>
-      </c>
-      <c r="D12" t="s" s="107">
-        <v>44</v>
-      </c>
-      <c r="F12" t="s" s="108">
-        <v>26</v>
-      </c>
-      <c r="G12" t="s" s="109">
+      <c r="C12" t="s" s="129">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s" s="130">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s" s="131">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s" s="132">
         <v>9</v>
       </c>
     </row>
@@ -4148,42 +4153,42 @@
       <c r="A13" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="B13" t="n" s="110">
+      <c r="B13" t="n" s="133">
         <v>4.0</v>
       </c>
-      <c r="C13" t="s" s="111">
-        <v>42</v>
-      </c>
-      <c r="D13" t="s" s="112">
-        <v>44</v>
-      </c>
-      <c r="F13" t="n" s="113">
+      <c r="C13" t="s" s="134">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s" s="135">
+        <v>36</v>
+      </c>
+      <c r="F13" t="n" s="136">
         <v>24.0</v>
       </c>
-      <c r="G13" t="n" s="114">
+      <c r="G13" t="n" s="137">
         <v>24.0</v>
       </c>
-      <c r="H13" t="s" s="115">
-        <v>24</v>
+      <c r="H13" t="n" s="139">
+        <v>1.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="B14" t="n" s="116">
+      <c r="B14" t="n" s="140">
         <v>5.0</v>
       </c>
-      <c r="C14" t="s" s="117">
-        <v>42</v>
-      </c>
-      <c r="D14" t="s" s="118">
-        <v>43</v>
-      </c>
-      <c r="E14" t="s" s="119">
-        <v>27</v>
-      </c>
-      <c r="G14" t="s" s="120">
+      <c r="C14" t="s" s="141">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s" s="142">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s" s="143">
+        <v>23</v>
+      </c>
+      <c r="G14" t="s" s="144">
         <v>9</v>
       </c>
     </row>
@@ -4191,19 +4196,19 @@
       <c r="A15" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="B15" t="n" s="121">
+      <c r="B15" t="n" s="145">
         <v>5.0</v>
       </c>
-      <c r="C15" t="s" s="122">
-        <v>42</v>
-      </c>
-      <c r="D15" t="s" s="123">
-        <v>43</v>
-      </c>
-      <c r="E15" t="s" s="124">
-        <v>28</v>
-      </c>
-      <c r="G15" t="s" s="125">
+      <c r="C15" t="s" s="146">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s" s="147">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s" s="148">
+        <v>24</v>
+      </c>
+      <c r="G15" t="s" s="149">
         <v>9</v>
       </c>
     </row>
@@ -4211,42 +4216,42 @@
       <c r="A16" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="B16" t="n" s="126">
+      <c r="B16" t="n" s="150">
         <v>5.0</v>
       </c>
-      <c r="C16" t="s" s="127">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s" s="128">
-        <v>43</v>
-      </c>
-      <c r="E16" t="n" s="129">
+      <c r="C16" t="s" s="151">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s" s="152">
+        <v>35</v>
+      </c>
+      <c r="E16" t="n" s="153">
         <v>15.0</v>
       </c>
-      <c r="G16" t="n" s="130">
+      <c r="G16" t="n" s="154">
         <v>15.0</v>
       </c>
-      <c r="H16" t="s" s="131">
-        <v>24</v>
+      <c r="H16" t="n" s="156">
+        <v>1.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="B17" t="n" s="132">
+      <c r="B17" t="n" s="157">
         <v>6.0</v>
       </c>
-      <c r="C17" t="s" s="133">
-        <v>42</v>
-      </c>
-      <c r="D17" t="s" s="134">
-        <v>44</v>
-      </c>
-      <c r="F17" t="s" s="135">
-        <v>29</v>
-      </c>
-      <c r="G17" t="s" s="136">
+      <c r="C17" t="s" s="158">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s" s="159">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s" s="160">
+        <v>25</v>
+      </c>
+      <c r="G17" t="s" s="161">
         <v>9</v>
       </c>
     </row>
@@ -4254,19 +4259,19 @@
       <c r="A18" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="B18" t="n" s="137">
+      <c r="B18" t="n" s="162">
         <v>6.0</v>
       </c>
-      <c r="C18" t="s" s="138">
-        <v>42</v>
-      </c>
-      <c r="D18" t="s" s="139">
-        <v>44</v>
-      </c>
-      <c r="F18" t="s" s="140">
-        <v>30</v>
-      </c>
-      <c r="G18" t="s" s="141">
+      <c r="C18" t="s" s="163">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s" s="164">
+        <v>36</v>
+      </c>
+      <c r="F18" t="s" s="165">
+        <v>26</v>
+      </c>
+      <c r="G18" t="s" s="166">
         <v>9</v>
       </c>
     </row>
@@ -4274,23 +4279,23 @@
       <c r="A19" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="B19" t="n" s="142">
+      <c r="B19" t="n" s="167">
         <v>6.0</v>
       </c>
-      <c r="C19" t="s" s="143">
-        <v>42</v>
-      </c>
-      <c r="D19" t="s" s="144">
-        <v>44</v>
-      </c>
-      <c r="F19" t="n" s="145">
+      <c r="C19" t="s" s="168">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s" s="169">
+        <v>36</v>
+      </c>
+      <c r="F19" t="n" s="170">
         <v>26.0</v>
       </c>
-      <c r="G19" t="n" s="146">
+      <c r="G19" t="n" s="171">
         <v>26.0</v>
       </c>
-      <c r="H19" t="s" s="147">
-        <v>24</v>
+      <c r="H19" t="n" s="173">
+        <v>1.0</v>
       </c>
     </row>
     <row r="20">
@@ -4301,22 +4306,22 @@
         <v>8.0</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" t="n" s="148">
+        <v>35</v>
+      </c>
+      <c r="E20" t="n" s="174">
         <v>15.0</v>
       </c>
-      <c r="F20" t="n" s="149">
+      <c r="F20" t="n" s="175">
         <v>88.0</v>
       </c>
-      <c r="G20" t="s" s="150">
-        <v>38</v>
-      </c>
-      <c r="H20" t="s" s="151">
-        <v>39</v>
+      <c r="G20" t="n" s="176">
+        <v>73.0</v>
+      </c>
+      <c r="H20" t="n" s="178">
+        <v>0.8295454545454546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Detailed report layout enhancements. * NullPointerException fix if join columns have null values.
</commit_message>
<xml_diff>
--- a/tests/data/desired/detailedreport.xlsx
+++ b/tests/data/desired/detailedreport.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="37">
   <si>
     <t>Column Name</t>
   </si>
@@ -1683,8 +1683,8 @@
       <c r="E23" t="n">
         <v>77.0</v>
       </c>
-      <c r="F23" t="n">
-        <v>0.0</v>
+      <c r="F23" t="s">
+        <v>28</v>
       </c>
       <c r="G23" t="s" s="5">
         <v>10</v>
@@ -2055,8 +2055,8 @@
       <c r="E17" t="n">
         <v>77.0</v>
       </c>
-      <c r="F17" t="n">
-        <v>0.0</v>
+      <c r="F17" t="s">
+        <v>28</v>
       </c>
       <c r="G17" t="s" s="5">
         <v>10</v>
@@ -2427,8 +2427,8 @@
       <c r="E17" t="n">
         <v>77.0</v>
       </c>
-      <c r="F17" t="n">
-        <v>0.0</v>
+      <c r="F17" t="s">
+        <v>28</v>
       </c>
       <c r="G17" t="s" s="5">
         <v>10</v>
@@ -2709,8 +2709,8 @@
       <c r="E11" t="n">
         <v>77.0</v>
       </c>
-      <c r="F11" t="n">
-        <v>0.0</v>
+      <c r="F11" t="s">
+        <v>28</v>
       </c>
       <c r="G11" t="s" s="5">
         <v>10</v>
@@ -2849,8 +2849,8 @@
       <c r="E23" t="n">
         <v>11.0</v>
       </c>
-      <c r="F23" t="n">
-        <v>0.0</v>
+      <c r="F23" t="s">
+        <v>28</v>
       </c>
       <c r="G23" t="s" s="5">
         <v>10</v>
@@ -2909,8 +2909,8 @@
       <c r="E26" t="n">
         <v>12.0</v>
       </c>
-      <c r="F26" t="n">
-        <v>0.0</v>
+      <c r="F26" t="s">
+        <v>28</v>
       </c>
       <c r="G26" t="s" s="5">
         <v>10</v>
@@ -2969,8 +2969,8 @@
       <c r="E29" t="n">
         <v>13.0</v>
       </c>
-      <c r="F29" t="n">
-        <v>0.0</v>
+      <c r="F29" t="s">
+        <v>28</v>
       </c>
       <c r="G29" t="s" s="5">
         <v>10</v>
@@ -3029,8 +3029,8 @@
       <c r="E32" t="n">
         <v>15.0</v>
       </c>
-      <c r="F32" t="n">
-        <v>0.0</v>
+      <c r="F32" t="s">
+        <v>28</v>
       </c>
       <c r="G32" t="s" s="5">
         <v>10</v>
@@ -3089,8 +3089,8 @@
       <c r="E35" t="n">
         <v>77.0</v>
       </c>
-      <c r="F35" t="n">
-        <v>0.0</v>
+      <c r="F35" t="s">
+        <v>28</v>
       </c>
       <c r="G35" t="s" s="5">
         <v>10</v>
@@ -3149,8 +3149,8 @@
       <c r="E38" t="n">
         <v>15.0</v>
       </c>
-      <c r="F38" t="n">
-        <v>0.0</v>
+      <c r="F38" t="s">
+        <v>28</v>
       </c>
       <c r="G38" t="s" s="5">
         <v>10</v>

</xml_diff>

<commit_message>
* Added the 'desc' attribute to <data-source> node that describes the data source in detailed join layout.
</commit_message>
<xml_diff>
--- a/tests/data/desired/detailedreport.xlsx
+++ b/tests/data/desired/detailedreport.xlsx
@@ -35,10 +35,10 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Source1</t>
+    <t>1st Source</t>
   </si>
   <si>
-    <t>Source2</t>
+    <t>2nd Source</t>
   </si>
   <si>
     <t>Difference</t>
@@ -1304,8 +1304,8 @@
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.78125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.9140625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="13.52734375" customWidth="true" bestFit="true"/>
   </cols>
@@ -1766,8 +1766,8 @@
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.78125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.9140625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="13.52734375" customWidth="true" bestFit="true"/>
   </cols>
@@ -2138,8 +2138,8 @@
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.78125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.9140625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="13.52734375" customWidth="true" bestFit="true"/>
   </cols>
@@ -2510,8 +2510,8 @@
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.78125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.9140625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="12.55078125" customWidth="true" bestFit="true"/>
   </cols>
@@ -3172,8 +3172,8 @@
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.78125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.9140625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="13.52734375" customWidth="true" bestFit="true"/>
   </cols>
@@ -3534,8 +3534,8 @@
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.78125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.9140625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="12.55078125" customWidth="true" bestFit="true"/>
   </cols>
@@ -3858,8 +3858,8 @@
     <col min="2" max="2" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="9.2578125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.1484375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.78125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="12.9140625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.75390625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="13.52734375" customWidth="true" bestFit="true"/>
   </cols>

</xml_diff>

<commit_message>
* Calculating the relative error to the value from the first data source result.
</commit_message>
<xml_diff>
--- a/tests/data/desired/detailedreport.xlsx
+++ b/tests/data/desired/detailedreport.xlsx
@@ -1307,7 +1307,7 @@
     <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="13.52734375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="13.7109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -1387,7 +1387,7 @@
         <v>10.0</v>
       </c>
       <c r="G5" t="n" s="4">
-        <v>0.47619047619047616</v>
+        <v>0.9090909090909091</v>
       </c>
     </row>
     <row r="6">
@@ -1447,7 +1447,7 @@
         <v>10.0</v>
       </c>
       <c r="G8" t="n" s="4">
-        <v>0.45454545454545453</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="9">
@@ -1747,7 +1747,7 @@
         <v>73.0</v>
       </c>
       <c r="G26" t="n" s="4">
-        <v>0.8295454545454546</v>
+        <v>4.866666666666666</v>
       </c>
     </row>
   </sheetData>
@@ -1769,7 +1769,7 @@
     <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="13.52734375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="13.7109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -1849,7 +1849,7 @@
         <v>10.0</v>
       </c>
       <c r="G5" t="n" s="5">
-        <v>0.47619047619047616</v>
+        <v>0.9090909090909091</v>
       </c>
     </row>
     <row r="6">
@@ -1909,7 +1909,7 @@
         <v>10.0</v>
       </c>
       <c r="G8" t="n" s="5">
-        <v>0.45454545454545453</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="9">
@@ -2119,7 +2119,7 @@
         <v>73.0</v>
       </c>
       <c r="G20" t="n" s="5">
-        <v>0.8295454545454546</v>
+        <v>4.866666666666666</v>
       </c>
     </row>
   </sheetData>
@@ -2141,7 +2141,7 @@
     <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="13.52734375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="13.7109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -2221,7 +2221,7 @@
         <v>10.0</v>
       </c>
       <c r="G5" t="n" s="5">
-        <v>0.47619047619047616</v>
+        <v>0.9090909090909091</v>
       </c>
     </row>
     <row r="6">
@@ -2281,7 +2281,7 @@
         <v>10.0</v>
       </c>
       <c r="G8" t="n" s="5">
-        <v>0.45454545454545453</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="9">
@@ -2491,7 +2491,7 @@
         <v>73.0</v>
       </c>
       <c r="G20" t="n" s="5">
-        <v>0.8295454545454546</v>
+        <v>4.866666666666666</v>
       </c>
     </row>
   </sheetData>
@@ -2513,7 +2513,7 @@
     <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="12.55078125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="13.7109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -2593,7 +2593,7 @@
         <v>10.0</v>
       </c>
       <c r="G5" t="n" s="5">
-        <v>0.47619047619047616</v>
+        <v>0.9090909090909091</v>
       </c>
     </row>
     <row r="6">
@@ -2653,7 +2653,7 @@
         <v>10.0</v>
       </c>
       <c r="G8" t="n" s="5">
-        <v>0.45454545454545453</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="9">
@@ -2773,7 +2773,7 @@
         <v>73.0</v>
       </c>
       <c r="G14" t="n" s="5">
-        <v>0.8295454545454546</v>
+        <v>4.866666666666666</v>
       </c>
     </row>
     <row r="20">
@@ -3175,7 +3175,7 @@
     <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="13.52734375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="13.7109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -3255,7 +3255,7 @@
         <v>10.0</v>
       </c>
       <c r="G5" t="n" s="4">
-        <v>0.47619047619047616</v>
+        <v>0.9090909090909091</v>
       </c>
     </row>
     <row r="6">
@@ -3315,7 +3315,7 @@
         <v>10.0</v>
       </c>
       <c r="G8" t="n" s="4">
-        <v>0.45454545454545453</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="9">
@@ -3515,7 +3515,7 @@
         <v>73.0</v>
       </c>
       <c r="G21" t="n" s="4">
-        <v>0.8295454545454546</v>
+        <v>4.866666666666666</v>
       </c>
     </row>
   </sheetData>
@@ -3537,7 +3537,7 @@
     <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="12.55078125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="13.7109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -3617,7 +3617,7 @@
         <v>10.0</v>
       </c>
       <c r="G5" t="n" s="20">
-        <v>0.47619047619047616</v>
+        <v>0.9090909090909091</v>
       </c>
     </row>
     <row r="6">
@@ -3677,7 +3677,7 @@
         <v>10.0</v>
       </c>
       <c r="G8" t="n" s="35">
-        <v>0.45454545454545453</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="9">
@@ -3697,7 +3697,7 @@
         <v>73.0</v>
       </c>
       <c r="G9" t="n" s="40">
-        <v>0.8295454545454546</v>
+        <v>4.866666666666666</v>
       </c>
     </row>
     <row r="10">
@@ -3757,7 +3757,7 @@
         <v>10.0</v>
       </c>
       <c r="G12" t="n" s="55">
-        <v>0.47619047619047616</v>
+        <v>0.9090909090909091</v>
       </c>
     </row>
     <row r="13">
@@ -3817,7 +3817,7 @@
         <v>10.0</v>
       </c>
       <c r="G15" t="n" s="70">
-        <v>0.45454545454545453</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="16">
@@ -3837,7 +3837,7 @@
         <v>73.0</v>
       </c>
       <c r="G16" t="n" s="75">
-        <v>0.8295454545454546</v>
+        <v>4.866666666666666</v>
       </c>
     </row>
   </sheetData>
@@ -3861,7 +3861,7 @@
     <col min="5" max="5" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.75390625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="13.52734375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.7109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3965,7 +3965,7 @@
         <v>10.0</v>
       </c>
       <c r="H4" t="n" s="90">
-        <v>0.47619047619047616</v>
+        <v>0.9090909090909091</v>
       </c>
     </row>
     <row r="5">
@@ -4043,7 +4043,7 @@
         <v>10.0</v>
       </c>
       <c r="H7" t="n" s="105">
-        <v>0.45454545454545453</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="8">
@@ -4321,7 +4321,7 @@
         <v>73.0</v>
       </c>
       <c r="H20" t="n" s="178">
-        <v>0.8295454545454546</v>
+        <v>4.866666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Added global ligreto parameters. * Added null and missing strings used instead of null values and missing rows.
</commit_message>
<xml_diff>
--- a/tests/data/desired/detailedreport.xlsx
+++ b/tests/data/desired/detailedreport.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="38">
   <si>
     <t>Column Name</t>
   </si>
@@ -89,6 +89,9 @@
     <t>1Martin3</t>
   </si>
   <si>
+    <t>&lt;missing&gt;</t>
+  </si>
+  <si>
     <t>1Velky3</t>
   </si>
   <si>
@@ -147,7 +150,7 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="151">
+  <fonts count="163">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -334,6 +337,78 @@
       <name val="Calibri"/>
       <sz val="11.0"/>
       <color rgb="20D020"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
       <u val="none"/>
     </font>
     <font>
@@ -1110,7 +1185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
@@ -1233,10 +1308,10 @@
     <xf numFmtId="0" fontId="96" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="97" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="98" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="98" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="99" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="100" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="101" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="101" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="102" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="103" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="104" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
@@ -1250,13 +1325,13 @@
     <xf numFmtId="0" fontId="112" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="113" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="114" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="114" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="115" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="116" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="117" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="118" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="119" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="120" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="120" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="121" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="122" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="123" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
@@ -1267,7 +1342,6 @@
     <xf numFmtId="0" fontId="128" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="129" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="130" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="130" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="131" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="132" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="133" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
@@ -1277,6 +1351,7 @@
     <xf numFmtId="0" fontId="137" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="138" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="139" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="139" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="140" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="141" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="142" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
@@ -1284,12 +1359,24 @@
     <xf numFmtId="0" fontId="144" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="145" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="146" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="146" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="147" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="148" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="149" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="150" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="150" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="151" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="152" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="153" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="154" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="155" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="156" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="157" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="158" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="158" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="159" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="160" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="161" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="162" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="162" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -1303,7 +1390,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
@@ -1460,6 +1547,9 @@
       <c r="D9" t="s" s="3">
         <v>19</v>
       </c>
+      <c r="E9" t="s" s="3">
+        <v>20</v>
+      </c>
       <c r="F9" t="s" s="3">
         <v>9</v>
       </c>
@@ -1472,6 +1562,9 @@
         <v>3.0</v>
       </c>
       <c r="D10" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s" s="3">
         <v>20</v>
       </c>
       <c r="F10" t="s" s="3">
@@ -1487,6 +1580,9 @@
       </c>
       <c r="D11" t="n" s="3">
         <v>13.0</v>
+      </c>
+      <c r="E11" t="s" s="3">
+        <v>20</v>
       </c>
       <c r="F11" t="n" s="3">
         <v>13.0</v>
@@ -1502,8 +1598,11 @@
       <c r="C12" t="n" s="3">
         <v>4.0</v>
       </c>
+      <c r="D12" t="s" s="3">
+        <v>20</v>
+      </c>
       <c r="E12" t="s" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s" s="3">
         <v>9</v>
@@ -1516,8 +1615,11 @@
       <c r="C13" t="n" s="3">
         <v>4.0</v>
       </c>
+      <c r="D13" t="s" s="3">
+        <v>20</v>
+      </c>
       <c r="E13" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F13" t="s" s="3">
         <v>9</v>
@@ -1529,6 +1631,9 @@
       </c>
       <c r="C14" t="n" s="3">
         <v>4.0</v>
+      </c>
+      <c r="D14" t="s" s="3">
+        <v>20</v>
       </c>
       <c r="E14" t="n" s="3">
         <v>24.0</v>
@@ -1548,7 +1653,10 @@
         <v>5.0</v>
       </c>
       <c r="D15" t="s" s="3">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="E15" t="s" s="3">
+        <v>20</v>
       </c>
       <c r="F15" t="s" s="3">
         <v>9</v>
@@ -1562,7 +1670,10 @@
         <v>5.0</v>
       </c>
       <c r="D16" t="s" s="3">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E16" t="s" s="3">
+        <v>20</v>
       </c>
       <c r="F16" t="s" s="3">
         <v>9</v>
@@ -1577,6 +1688,9 @@
       </c>
       <c r="D17" t="n" s="3">
         <v>15.0</v>
+      </c>
+      <c r="E17" t="s" s="3">
+        <v>20</v>
       </c>
       <c r="F17" t="n" s="3">
         <v>15.0</v>
@@ -1592,8 +1706,11 @@
       <c r="C18" t="n" s="3">
         <v>6.0</v>
       </c>
+      <c r="D18" t="s" s="3">
+        <v>20</v>
+      </c>
       <c r="E18" t="s" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F18" t="s" s="3">
         <v>9</v>
@@ -1606,8 +1723,11 @@
       <c r="C19" t="n" s="3">
         <v>6.0</v>
       </c>
+      <c r="D19" t="s" s="3">
+        <v>20</v>
+      </c>
       <c r="E19" t="s" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F19" t="s" s="3">
         <v>9</v>
@@ -1619,6 +1739,9 @@
       </c>
       <c r="C20" t="n" s="3">
         <v>6.0</v>
+      </c>
+      <c r="D20" t="s" s="3">
+        <v>20</v>
       </c>
       <c r="E20" t="n" s="3">
         <v>26.0</v>
@@ -1638,13 +1761,13 @@
         <v>7.0</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G21" t="s" s="5">
         <v>10</v>
@@ -1658,13 +1781,13 @@
         <v>7.0</v>
       </c>
       <c r="D22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" t="s">
         <v>29</v>
-      </c>
-      <c r="E22" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" t="s">
-        <v>28</v>
       </c>
       <c r="G22" t="s" s="5">
         <v>10</v>
@@ -1684,7 +1807,7 @@
         <v>77.0</v>
       </c>
       <c r="F23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G23" t="s" s="5">
         <v>10</v>
@@ -1698,13 +1821,13 @@
         <v>8.0</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G24" t="s" s="5">
         <v>10</v>
@@ -1718,13 +1841,13 @@
         <v>8.0</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G25" t="s" s="5">
         <v>10</v>
@@ -1765,7 +1888,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
@@ -1922,6 +2045,9 @@
       <c r="D9" t="s">
         <v>19</v>
       </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
       <c r="F9" t="s">
         <v>9</v>
       </c>
@@ -1934,6 +2060,9 @@
         <v>3.0</v>
       </c>
       <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
         <v>20</v>
       </c>
       <c r="F10" t="s">
@@ -1949,6 +2078,9 @@
       </c>
       <c r="D11" t="n">
         <v>13.0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
       </c>
       <c r="F11" t="n">
         <v>13.0</v>
@@ -1965,7 +2097,10 @@
         <v>5.0</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
       </c>
       <c r="F12" t="s">
         <v>9</v>
@@ -1979,7 +2114,10 @@
         <v>5.0</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
       </c>
       <c r="F13" t="s">
         <v>9</v>
@@ -1994,6 +2132,9 @@
       </c>
       <c r="D14" t="n">
         <v>15.0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
       </c>
       <c r="F14" t="n">
         <v>15.0</v>
@@ -2010,13 +2151,13 @@
         <v>7.0</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G15" t="s" s="5">
         <v>10</v>
@@ -2030,13 +2171,13 @@
         <v>7.0</v>
       </c>
       <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" t="s">
         <v>29</v>
-      </c>
-      <c r="E16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" t="s">
-        <v>28</v>
       </c>
       <c r="G16" t="s" s="5">
         <v>10</v>
@@ -2056,7 +2197,7 @@
         <v>77.0</v>
       </c>
       <c r="F17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G17" t="s" s="5">
         <v>10</v>
@@ -2070,13 +2211,13 @@
         <v>8.0</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G18" t="s" s="5">
         <v>10</v>
@@ -2090,13 +2231,13 @@
         <v>8.0</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G19" t="s" s="5">
         <v>10</v>
@@ -2137,7 +2278,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
@@ -2291,8 +2432,11 @@
       <c r="C9" t="n">
         <v>4.0</v>
       </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
         <v>9</v>
@@ -2305,8 +2449,11 @@
       <c r="C10" t="n">
         <v>4.0</v>
       </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
@@ -2318,6 +2465,9 @@
       </c>
       <c r="C11" t="n">
         <v>4.0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
       </c>
       <c r="E11" t="n">
         <v>24.0</v>
@@ -2336,8 +2486,11 @@
       <c r="C12" t="n">
         <v>6.0</v>
       </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F12" t="s">
         <v>9</v>
@@ -2350,8 +2503,11 @@
       <c r="C13" t="n">
         <v>6.0</v>
       </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
         <v>9</v>
@@ -2363,6 +2519,9 @@
       </c>
       <c r="C14" t="n">
         <v>6.0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
       </c>
       <c r="E14" t="n">
         <v>26.0</v>
@@ -2382,13 +2541,13 @@
         <v>7.0</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G15" t="s" s="5">
         <v>10</v>
@@ -2402,13 +2561,13 @@
         <v>7.0</v>
       </c>
       <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" t="s">
         <v>29</v>
-      </c>
-      <c r="E16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" t="s">
-        <v>28</v>
       </c>
       <c r="G16" t="s" s="5">
         <v>10</v>
@@ -2428,7 +2587,7 @@
         <v>77.0</v>
       </c>
       <c r="F17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G17" t="s" s="5">
         <v>10</v>
@@ -2442,13 +2601,13 @@
         <v>8.0</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G18" t="s" s="5">
         <v>10</v>
@@ -2462,13 +2621,13 @@
         <v>8.0</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G19" t="s" s="5">
         <v>10</v>
@@ -2509,7 +2668,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
@@ -2664,13 +2823,13 @@
         <v>7.0</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G9" t="s" s="5">
         <v>10</v>
@@ -2684,13 +2843,13 @@
         <v>7.0</v>
       </c>
       <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
         <v>29</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" t="s">
-        <v>28</v>
       </c>
       <c r="G10" t="s" s="5">
         <v>10</v>
@@ -2710,7 +2869,7 @@
         <v>77.0</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G11" t="s" s="5">
         <v>10</v>
@@ -2724,13 +2883,13 @@
         <v>8.0</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G12" t="s" s="5">
         <v>10</v>
@@ -2744,13 +2903,13 @@
         <v>8.0</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G13" t="s" s="5">
         <v>10</v>
@@ -2810,7 +2969,7 @@
         <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G21" t="s" s="5">
         <v>10</v>
@@ -2830,7 +2989,7 @@
         <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G22" t="s" s="5">
         <v>10</v>
@@ -2850,7 +3009,7 @@
         <v>11.0</v>
       </c>
       <c r="F23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G23" t="s" s="5">
         <v>10</v>
@@ -2870,7 +3029,7 @@
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G24" t="s" s="5">
         <v>10</v>
@@ -2890,7 +3049,7 @@
         <v>17</v>
       </c>
       <c r="F25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G25" t="s" s="5">
         <v>10</v>
@@ -2910,7 +3069,7 @@
         <v>12.0</v>
       </c>
       <c r="F26" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G26" t="s" s="5">
         <v>10</v>
@@ -2930,7 +3089,7 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G27" t="s" s="5">
         <v>10</v>
@@ -2944,13 +3103,13 @@
         <v>3.0</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E28" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G28" t="s" s="5">
         <v>10</v>
@@ -2970,7 +3129,7 @@
         <v>13.0</v>
       </c>
       <c r="F29" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G29" t="s" s="5">
         <v>10</v>
@@ -2984,13 +3143,13 @@
         <v>5.0</v>
       </c>
       <c r="D30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F30" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G30" t="s" s="5">
         <v>10</v>
@@ -3004,13 +3163,13 @@
         <v>5.0</v>
       </c>
       <c r="D31" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E31" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G31" t="s" s="5">
         <v>10</v>
@@ -3030,7 +3189,7 @@
         <v>15.0</v>
       </c>
       <c r="F32" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G32" t="s" s="5">
         <v>10</v>
@@ -3044,13 +3203,13 @@
         <v>7.0</v>
       </c>
       <c r="D33" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E33" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F33" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G33" t="s" s="5">
         <v>10</v>
@@ -3064,13 +3223,13 @@
         <v>7.0</v>
       </c>
       <c r="D34" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" t="s">
         <v>29</v>
-      </c>
-      <c r="E34" t="s">
-        <v>29</v>
-      </c>
-      <c r="F34" t="s">
-        <v>28</v>
       </c>
       <c r="G34" t="s" s="5">
         <v>10</v>
@@ -3090,7 +3249,7 @@
         <v>77.0</v>
       </c>
       <c r="F35" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G35" t="s" s="5">
         <v>10</v>
@@ -3104,13 +3263,13 @@
         <v>8.0</v>
       </c>
       <c r="D36" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E36" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F36" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G36" t="s" s="5">
         <v>10</v>
@@ -3124,13 +3283,13 @@
         <v>8.0</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E37" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F37" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G37" t="s" s="5">
         <v>10</v>
@@ -3150,7 +3309,7 @@
         <v>15.0</v>
       </c>
       <c r="F38" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G38" t="s" s="5">
         <v>10</v>
@@ -3171,7 +3330,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
@@ -3328,6 +3487,9 @@
       <c r="D9" t="s" s="3">
         <v>19</v>
       </c>
+      <c r="E9" t="s" s="3">
+        <v>20</v>
+      </c>
       <c r="F9" t="s" s="3">
         <v>9</v>
       </c>
@@ -3340,6 +3502,9 @@
         <v>3.0</v>
       </c>
       <c r="D10" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s" s="3">
         <v>20</v>
       </c>
       <c r="F10" t="s" s="3">
@@ -3355,6 +3520,9 @@
       </c>
       <c r="D11" t="n" s="3">
         <v>13.0</v>
+      </c>
+      <c r="E11" t="s" s="3">
+        <v>20</v>
       </c>
       <c r="F11" t="n" s="3">
         <v>13.0</v>
@@ -3370,8 +3538,11 @@
       <c r="C12" t="n" s="3">
         <v>4.0</v>
       </c>
+      <c r="D12" t="s" s="3">
+        <v>20</v>
+      </c>
       <c r="E12" t="s" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s" s="3">
         <v>9</v>
@@ -3384,8 +3555,11 @@
       <c r="C13" t="n" s="3">
         <v>4.0</v>
       </c>
+      <c r="D13" t="s" s="3">
+        <v>20</v>
+      </c>
       <c r="E13" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F13" t="s" s="3">
         <v>9</v>
@@ -3397,6 +3571,9 @@
       </c>
       <c r="C14" t="n" s="3">
         <v>4.0</v>
+      </c>
+      <c r="D14" t="s" s="3">
+        <v>20</v>
       </c>
       <c r="E14" t="n" s="3">
         <v>24.0</v>
@@ -3416,7 +3593,10 @@
         <v>5.0</v>
       </c>
       <c r="D15" t="s" s="3">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="E15" t="s" s="3">
+        <v>20</v>
       </c>
       <c r="F15" t="s" s="3">
         <v>9</v>
@@ -3430,7 +3610,10 @@
         <v>5.0</v>
       </c>
       <c r="D16" t="s" s="3">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E16" t="s" s="3">
+        <v>20</v>
       </c>
       <c r="F16" t="s" s="3">
         <v>9</v>
@@ -3445,6 +3628,9 @@
       </c>
       <c r="D17" t="n" s="3">
         <v>15.0</v>
+      </c>
+      <c r="E17" t="s" s="3">
+        <v>20</v>
       </c>
       <c r="F17" t="n" s="3">
         <v>15.0</v>
@@ -3460,8 +3646,11 @@
       <c r="C18" t="n" s="3">
         <v>6.0</v>
       </c>
+      <c r="D18" t="s" s="3">
+        <v>20</v>
+      </c>
       <c r="E18" t="s" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F18" t="s" s="3">
         <v>9</v>
@@ -3474,8 +3663,11 @@
       <c r="C19" t="n" s="3">
         <v>6.0</v>
       </c>
+      <c r="D19" t="s" s="3">
+        <v>20</v>
+      </c>
       <c r="E19" t="s" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F19" t="s" s="3">
         <v>9</v>
@@ -3487,6 +3679,9 @@
       </c>
       <c r="C20" t="n" s="3">
         <v>6.0</v>
+      </c>
+      <c r="D20" t="s" s="3">
+        <v>20</v>
       </c>
       <c r="E20" t="n" s="3">
         <v>26.0</v>
@@ -3533,7 +3728,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
@@ -3855,7 +4050,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="18.234375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="7.01171875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="8.0" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="9.2578125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.1484375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="14.7578125" customWidth="true" bestFit="true"/>
@@ -3872,10 +4067,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s" s="1">
         <v>2</v>
@@ -3898,10 +4093,10 @@
         <v>1.0</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s" s="76">
         <v>7</v>
@@ -3924,10 +4119,10 @@
         <v>1.0</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s" s="81">
         <v>12</v>
@@ -3950,10 +4145,10 @@
         <v>1.0</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E4" t="n" s="86">
         <v>11.0</v>
@@ -3976,10 +4171,10 @@
         <v>2.0</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s" s="91">
         <v>15</v>
@@ -4002,10 +4197,10 @@
         <v>2.0</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s" s="96">
         <v>17</v>
@@ -4028,10 +4223,10 @@
         <v>2.0</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E7" t="n" s="101">
         <v>12.0</v>
@@ -4054,15 +4249,18 @@
         <v>3.0</v>
       </c>
       <c r="C8" t="s" s="107">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s" s="108">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s" s="109">
         <v>19</v>
       </c>
-      <c r="G8" t="s" s="110">
+      <c r="F8" t="s" s="110">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s" s="111">
         <v>9</v>
       </c>
     </row>
@@ -4070,19 +4268,22 @@
       <c r="A9" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="B9" t="n" s="111">
+      <c r="B9" t="n" s="112">
         <v>3.0</v>
       </c>
-      <c r="C9" t="s" s="112">
-        <v>34</v>
-      </c>
-      <c r="D9" t="s" s="113">
+      <c r="C9" t="s" s="113">
         <v>35</v>
       </c>
-      <c r="E9" t="s" s="114">
-        <v>20</v>
-      </c>
-      <c r="G9" t="s" s="115">
+      <c r="D9" t="s" s="114">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s" s="115">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s" s="116">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s" s="117">
         <v>9</v>
       </c>
     </row>
@@ -4090,22 +4291,25 @@
       <c r="A10" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="B10" t="n" s="116">
+      <c r="B10" t="n" s="118">
         <v>3.0</v>
       </c>
-      <c r="C10" t="s" s="117">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s" s="118">
+      <c r="C10" t="s" s="119">
         <v>35</v>
       </c>
-      <c r="E10" t="n" s="119">
+      <c r="D10" t="s" s="120">
+        <v>36</v>
+      </c>
+      <c r="E10" t="n" s="121">
         <v>13.0</v>
       </c>
-      <c r="G10" t="n" s="120">
+      <c r="F10" t="s" s="122">
+        <v>20</v>
+      </c>
+      <c r="G10" t="n" s="123">
         <v>13.0</v>
       </c>
-      <c r="H10" t="n" s="122">
+      <c r="H10" t="n" s="125">
         <v>1.0</v>
       </c>
     </row>
@@ -4113,19 +4317,22 @@
       <c r="A11" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="B11" t="n" s="123">
+      <c r="B11" t="n" s="126">
         <v>4.0</v>
       </c>
-      <c r="C11" t="s" s="124">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s" s="125">
-        <v>36</v>
-      </c>
-      <c r="F11" t="s" s="126">
-        <v>21</v>
-      </c>
-      <c r="G11" t="s" s="127">
+      <c r="C11" t="s" s="127">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s" s="128">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s" s="129">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s" s="130">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s" s="131">
         <v>9</v>
       </c>
     </row>
@@ -4133,19 +4340,22 @@
       <c r="A12" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="B12" t="n" s="128">
+      <c r="B12" t="n" s="132">
         <v>4.0</v>
       </c>
-      <c r="C12" t="s" s="129">
-        <v>34</v>
-      </c>
-      <c r="D12" t="s" s="130">
-        <v>36</v>
-      </c>
-      <c r="F12" t="s" s="131">
-        <v>22</v>
-      </c>
-      <c r="G12" t="s" s="132">
+      <c r="C12" t="s" s="133">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s" s="134">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s" s="135">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s" s="136">
+        <v>23</v>
+      </c>
+      <c r="G12" t="s" s="137">
         <v>9</v>
       </c>
     </row>
@@ -4153,22 +4363,25 @@
       <c r="A13" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="B13" t="n" s="133">
+      <c r="B13" t="n" s="138">
         <v>4.0</v>
       </c>
-      <c r="C13" t="s" s="134">
-        <v>34</v>
-      </c>
-      <c r="D13" t="s" s="135">
-        <v>36</v>
-      </c>
-      <c r="F13" t="n" s="136">
+      <c r="C13" t="s" s="139">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s" s="140">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s" s="141">
+        <v>20</v>
+      </c>
+      <c r="F13" t="n" s="142">
         <v>24.0</v>
       </c>
-      <c r="G13" t="n" s="137">
+      <c r="G13" t="n" s="143">
         <v>24.0</v>
       </c>
-      <c r="H13" t="n" s="139">
+      <c r="H13" t="n" s="145">
         <v>1.0</v>
       </c>
     </row>
@@ -4176,19 +4389,22 @@
       <c r="A14" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="B14" t="n" s="140">
+      <c r="B14" t="n" s="146">
         <v>5.0</v>
       </c>
-      <c r="C14" t="s" s="141">
-        <v>34</v>
-      </c>
-      <c r="D14" t="s" s="142">
+      <c r="C14" t="s" s="147">
         <v>35</v>
       </c>
-      <c r="E14" t="s" s="143">
-        <v>23</v>
-      </c>
-      <c r="G14" t="s" s="144">
+      <c r="D14" t="s" s="148">
+        <v>36</v>
+      </c>
+      <c r="E14" t="s" s="149">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s" s="150">
+        <v>20</v>
+      </c>
+      <c r="G14" t="s" s="151">
         <v>9</v>
       </c>
     </row>
@@ -4196,19 +4412,22 @@
       <c r="A15" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="B15" t="n" s="145">
+      <c r="B15" t="n" s="152">
         <v>5.0</v>
       </c>
-      <c r="C15" t="s" s="146">
-        <v>34</v>
-      </c>
-      <c r="D15" t="s" s="147">
+      <c r="C15" t="s" s="153">
         <v>35</v>
       </c>
-      <c r="E15" t="s" s="148">
-        <v>24</v>
-      </c>
-      <c r="G15" t="s" s="149">
+      <c r="D15" t="s" s="154">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s" s="155">
+        <v>25</v>
+      </c>
+      <c r="F15" t="s" s="156">
+        <v>20</v>
+      </c>
+      <c r="G15" t="s" s="157">
         <v>9</v>
       </c>
     </row>
@@ -4216,22 +4435,25 @@
       <c r="A16" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="B16" t="n" s="150">
+      <c r="B16" t="n" s="158">
         <v>5.0</v>
       </c>
-      <c r="C16" t="s" s="151">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s" s="152">
+      <c r="C16" t="s" s="159">
         <v>35</v>
       </c>
-      <c r="E16" t="n" s="153">
+      <c r="D16" t="s" s="160">
+        <v>36</v>
+      </c>
+      <c r="E16" t="n" s="161">
         <v>15.0</v>
       </c>
-      <c r="G16" t="n" s="154">
+      <c r="F16" t="s" s="162">
+        <v>20</v>
+      </c>
+      <c r="G16" t="n" s="163">
         <v>15.0</v>
       </c>
-      <c r="H16" t="n" s="156">
+      <c r="H16" t="n" s="165">
         <v>1.0</v>
       </c>
     </row>
@@ -4239,19 +4461,22 @@
       <c r="A17" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="B17" t="n" s="157">
+      <c r="B17" t="n" s="166">
         <v>6.0</v>
       </c>
-      <c r="C17" t="s" s="158">
-        <v>34</v>
-      </c>
-      <c r="D17" t="s" s="159">
-        <v>36</v>
-      </c>
-      <c r="F17" t="s" s="160">
-        <v>25</v>
-      </c>
-      <c r="G17" t="s" s="161">
+      <c r="C17" t="s" s="167">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s" s="168">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s" s="169">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s" s="170">
+        <v>26</v>
+      </c>
+      <c r="G17" t="s" s="171">
         <v>9</v>
       </c>
     </row>
@@ -4259,19 +4484,22 @@
       <c r="A18" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="B18" t="n" s="162">
+      <c r="B18" t="n" s="172">
         <v>6.0</v>
       </c>
-      <c r="C18" t="s" s="163">
-        <v>34</v>
-      </c>
-      <c r="D18" t="s" s="164">
-        <v>36</v>
-      </c>
-      <c r="F18" t="s" s="165">
-        <v>26</v>
-      </c>
-      <c r="G18" t="s" s="166">
+      <c r="C18" t="s" s="173">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s" s="174">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s" s="175">
+        <v>20</v>
+      </c>
+      <c r="F18" t="s" s="176">
+        <v>27</v>
+      </c>
+      <c r="G18" t="s" s="177">
         <v>9</v>
       </c>
     </row>
@@ -4279,22 +4507,25 @@
       <c r="A19" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="B19" t="n" s="167">
+      <c r="B19" t="n" s="178">
         <v>6.0</v>
       </c>
-      <c r="C19" t="s" s="168">
-        <v>34</v>
-      </c>
-      <c r="D19" t="s" s="169">
-        <v>36</v>
-      </c>
-      <c r="F19" t="n" s="170">
+      <c r="C19" t="s" s="179">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s" s="180">
+        <v>37</v>
+      </c>
+      <c r="E19" t="s" s="181">
+        <v>20</v>
+      </c>
+      <c r="F19" t="n" s="182">
         <v>26.0</v>
       </c>
-      <c r="G19" t="n" s="171">
+      <c r="G19" t="n" s="183">
         <v>26.0</v>
       </c>
-      <c r="H19" t="n" s="173">
+      <c r="H19" t="n" s="185">
         <v>1.0</v>
       </c>
     </row>
@@ -4306,21 +4537,21 @@
         <v>8.0</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" t="n" s="174">
+        <v>36</v>
+      </c>
+      <c r="E20" t="n" s="186">
         <v>15.0</v>
       </c>
-      <c r="F20" t="n" s="175">
+      <c r="F20" t="n" s="187">
         <v>88.0</v>
       </c>
-      <c r="G20" t="n" s="176">
+      <c r="G20" t="n" s="188">
         <v>73.0</v>
       </c>
-      <c r="H20" t="n" s="178">
+      <c r="H20" t="n" s="190">
         <v>4.866666666666666</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* Tested the support for columns attribute in <comparison> node.
</commit_message>
<xml_diff>
--- a/tests/data/desired/detailedreport.xlsx
+++ b/tests/data/desired/detailedreport.xlsx
@@ -1390,7 +1390,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
@@ -1888,7 +1888,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
@@ -2278,7 +2278,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
@@ -2668,7 +2668,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
@@ -3330,7 +3330,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
@@ -3728,7 +3728,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
@@ -4050,7 +4050,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="18.234375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="8.0" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="9.2578125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.1484375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="14.7578125" customWidth="true" bestFit="true"/>

</xml_diff>